<commit_message>
Changement du fonctionnement du dico
</commit_message>
<xml_diff>
--- a/uploads/Conditions precedents to be satisfied on or before May 29, 2014.xlsx
+++ b/uploads/Conditions precedents to be satisfied on or before May 29, 2014.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="12240" windowHeight="7995"/>
@@ -2493,11 +2493,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3134,52 +3134,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3207,9 +3168,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3234,9 +3192,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3249,211 +3204,256 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3629,6 +3629,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3663,6 +3664,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3838,30 +3840,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="30" customWidth="1"/>
-    <col min="2" max="4" width="38.42578125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="20" style="30" customWidth="1"/>
-    <col min="6" max="6" width="52.5703125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="30" customWidth="1"/>
-    <col min="8" max="8" width="18" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="30" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="30" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="30" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" style="30" customWidth="1"/>
-    <col min="13" max="13" width="29.28515625" style="30" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="30"/>
+    <col min="1" max="1" width="37.85546875" style="17" customWidth="1"/>
+    <col min="2" max="4" width="38.42578125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="20" style="17" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="18" style="17" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="17" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" style="17" customWidth="1"/>
+    <col min="13" max="13" width="29.28515625" style="17" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3876,7 +3878,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1">
+    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3891,2281 +3893,2464 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="77.25" customHeight="1" thickBot="1"/>
-    <row r="4" spans="1:13" s="12" customFormat="1" ht="33" customHeight="1" thickBot="1">
-      <c r="A4" s="6" t="s">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:13" s="6" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7" t="s">
+      <c r="J4" s="106"/>
+      <c r="K4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="102" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="12" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="19" t="s">
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="105"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="21" t="s">
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+    </row>
+    <row r="6" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="24" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="26" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="29"/>
-    </row>
-    <row r="7" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="22" t="s">
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="101"/>
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="37"/>
-    </row>
-    <row r="8" spans="1:13" ht="107.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="31"/>
-      <c r="B8" s="22" t="s">
+      <c r="F7" s="20"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="23"/>
+    </row>
+    <row r="8" spans="1:13" ht="107.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="101"/>
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
-    </row>
-    <row r="9" spans="1:13" ht="52.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="31"/>
-      <c r="B9" s="22" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="23"/>
+    </row>
+    <row r="9" spans="1:13" ht="52.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="101"/>
+      <c r="B9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-    </row>
-    <row r="10" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A10" s="40"/>
-      <c r="B10" s="22" t="s">
+      <c r="F9" s="24"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="23"/>
+    </row>
+    <row r="10" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="84"/>
+      <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="34" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="44"/>
-    </row>
-    <row r="11" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="21" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="29"/>
+    </row>
+    <row r="11" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="46" t="s">
+      <c r="F11" s="20"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48" t="s">
+      <c r="J11" s="30"/>
+      <c r="K11" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="36"/>
-      <c r="M11" s="49"/>
-    </row>
-    <row r="12" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
-      <c r="A12" s="31"/>
-      <c r="B12" s="50" t="s">
+      <c r="L11" s="22"/>
+      <c r="M11" s="52"/>
+    </row>
+    <row r="12" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="101"/>
+      <c r="B12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="34" t="s">
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="54"/>
-    </row>
-    <row r="13" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A13" s="31"/>
-      <c r="B13" s="22" t="s">
+      <c r="F12" s="24"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="64"/>
+    </row>
+    <row r="13" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="101"/>
+      <c r="B13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="39" t="s">
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="54"/>
-    </row>
-    <row r="14" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A14" s="40"/>
-      <c r="B14" s="22" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="64"/>
+    </row>
+    <row r="14" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="84"/>
+      <c r="B14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="39" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="57"/>
-    </row>
-    <row r="15" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A15" s="58" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="65"/>
+    </row>
+    <row r="15" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="48" t="s">
+      <c r="F15" s="25"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="59"/>
-      <c r="K15" s="48" t="s">
+      <c r="J15" s="80"/>
+      <c r="K15" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="49"/>
-    </row>
-    <row r="16" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A16" s="60"/>
-      <c r="B16" s="22" t="s">
+      <c r="L15" s="22"/>
+      <c r="M15" s="52"/>
+    </row>
+    <row r="16" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="99"/>
+      <c r="B16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="39" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="54"/>
-    </row>
-    <row r="17" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
-      <c r="A17" s="60"/>
-      <c r="B17" s="50" t="s">
+      <c r="F16" s="25"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="64"/>
+    </row>
+    <row r="17" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="99"/>
+      <c r="B17" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="39" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="54"/>
-    </row>
-    <row r="18" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A18" s="60"/>
-      <c r="B18" s="22" t="s">
+      <c r="F17" s="25"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="64"/>
+    </row>
+    <row r="18" spans="1:13" ht="93" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="99"/>
+      <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="39" t="s">
+      <c r="C18" s="49"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="54"/>
-    </row>
-    <row r="19" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A19" s="62"/>
-      <c r="B19" s="22" t="s">
+      <c r="F18" s="25"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="64"/>
+    </row>
+    <row r="19" spans="1:13" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="100"/>
+      <c r="B19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="39" t="s">
+      <c r="C19" s="68"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="63"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="57"/>
-    </row>
-    <row r="20" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A20" s="65" t="s">
+      <c r="F19" s="25"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="65"/>
+    </row>
+    <row r="20" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="48" t="s">
+      <c r="F20" s="25"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="46" t="s">
+      <c r="J20" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="L20" s="36"/>
-      <c r="M20" s="49"/>
-    </row>
-    <row r="21" spans="1:13" ht="61.5" thickTop="1" thickBot="1">
-      <c r="A21" s="67"/>
-      <c r="B21" s="50" t="s">
+      <c r="L20" s="22"/>
+      <c r="M20" s="52"/>
+    </row>
+    <row r="21" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="93"/>
+      <c r="B21" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="54"/>
-    </row>
-    <row r="22" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A22" s="67"/>
-      <c r="B22" s="50" t="s">
+      <c r="C21" s="49"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="64"/>
+    </row>
+    <row r="22" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="93"/>
+      <c r="B22" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="54"/>
-    </row>
-    <row r="23" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
-      <c r="A23" s="69"/>
-      <c r="B23" s="50" t="s">
+      <c r="C22" s="49"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="64"/>
+    </row>
+    <row r="23" spans="1:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="94"/>
+      <c r="B23" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="57"/>
-    </row>
-    <row r="24" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A24" s="71" t="s">
+      <c r="C23" s="68"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="65"/>
+    </row>
+    <row r="24" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="48" t="s">
+      <c r="F24" s="25"/>
+      <c r="G24" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I24" s="72" t="s">
+      <c r="I24" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="46"/>
-      <c r="K24" s="48" t="s">
+      <c r="J24" s="67"/>
+      <c r="K24" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="36"/>
-      <c r="M24" s="49"/>
-    </row>
-    <row r="25" spans="1:13" ht="76.5" thickTop="1" thickBot="1">
-      <c r="A25" s="73"/>
-      <c r="B25" s="50" t="s">
+      <c r="L24" s="22"/>
+      <c r="M24" s="52"/>
+    </row>
+    <row r="25" spans="1:13" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="90"/>
+      <c r="B25" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="39" t="s">
+      <c r="C25" s="49"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="34" t="s">
+      <c r="F25" s="25"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I25" s="74"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="54"/>
-    </row>
-    <row r="26" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A26" s="73"/>
-      <c r="B26" s="22" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="64"/>
+    </row>
+    <row r="26" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="90"/>
+      <c r="B26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="39" t="s">
+      <c r="C26" s="49"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="34" t="s">
+      <c r="F26" s="25"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="74"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="54"/>
-    </row>
-    <row r="27" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A27" s="75"/>
-      <c r="B27" s="22" t="s">
+      <c r="I26" s="48"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="64"/>
+    </row>
+    <row r="27" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="91"/>
+      <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="39" t="s">
+      <c r="C27" s="68"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="39"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="34" t="s">
+      <c r="F27" s="25"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="76"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="57"/>
-    </row>
-    <row r="28" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A28" s="21" t="s">
+      <c r="I27" s="74"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="65"/>
+    </row>
+    <row r="28" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="77" t="s">
+      <c r="B28" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="45"/>
-      <c r="G28" s="48" t="s">
+      <c r="F28" s="57"/>
+      <c r="G28" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="78" t="s">
+      <c r="H28" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="79" t="s">
+      <c r="I28" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="J28" s="80" t="s">
+      <c r="J28" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="K28" s="48" t="s">
+      <c r="K28" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="49"/>
-    </row>
-    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A29" s="40"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="82"/>
-      <c r="J29" s="83"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="57"/>
-    </row>
-    <row r="30" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A30" s="84" t="s">
+      <c r="L28" s="22"/>
+      <c r="M28" s="52"/>
+    </row>
+    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="84"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="65"/>
+    </row>
+    <row r="30" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="78" t="s">
+      <c r="F30" s="57"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="48" t="s">
+      <c r="I30" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48" t="s">
+      <c r="J30" s="56"/>
+      <c r="K30" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="L30" s="36"/>
-      <c r="M30" s="49"/>
-    </row>
-    <row r="31" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A31" s="85"/>
-      <c r="B31" s="50" t="s">
+      <c r="L30" s="22"/>
+      <c r="M30" s="52"/>
+    </row>
+    <row r="31" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="66"/>
+      <c r="B31" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="39" t="s">
+      <c r="C31" s="49"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="54"/>
-    </row>
-    <row r="32" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A32" s="85"/>
-      <c r="B32" s="50" t="s">
+      <c r="F31" s="57"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="64"/>
+    </row>
+    <row r="32" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="66"/>
+      <c r="B32" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="39" t="s">
+      <c r="C32" s="49"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="45"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="54"/>
-    </row>
-    <row r="33" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A33" s="85"/>
-      <c r="B33" s="22" t="s">
+      <c r="F32" s="57"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="64"/>
+    </row>
+    <row r="33" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="66"/>
+      <c r="B33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="39" t="s">
+      <c r="C33" s="49"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="57"/>
-    </row>
-    <row r="34" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A34" s="86"/>
-      <c r="B34" s="22" t="s">
+      <c r="F33" s="57"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="65"/>
+    </row>
+    <row r="34" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="72"/>
+      <c r="B34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="55"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="39" t="s">
+      <c r="C34" s="68"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="45"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="44"/>
-    </row>
-    <row r="35" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A35" s="84" t="s">
+      <c r="F34" s="57"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="29"/>
+    </row>
+    <row r="35" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="46" t="s">
+      <c r="C35" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="48" t="s">
+      <c r="D35" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="39" t="s">
+      <c r="E35" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="78" t="s">
+      <c r="F35" s="57"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I35" s="48" t="s">
+      <c r="I35" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48" t="s">
+      <c r="J35" s="56"/>
+      <c r="K35" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="L35" s="36"/>
-      <c r="M35" s="49"/>
-    </row>
-    <row r="36" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A36" s="85"/>
-      <c r="B36" s="22" t="s">
+      <c r="L35" s="22"/>
+      <c r="M35" s="52"/>
+    </row>
+    <row r="36" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="66"/>
+      <c r="B36" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="39" t="s">
+      <c r="C36" s="49"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="45"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="54"/>
-    </row>
-    <row r="37" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A37" s="86"/>
-      <c r="B37" s="22" t="s">
+      <c r="F36" s="57"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="64"/>
+    </row>
+    <row r="37" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="72"/>
+      <c r="B37" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="39" t="s">
+      <c r="C37" s="68"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="45"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
-      <c r="K37" s="63"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="57"/>
-    </row>
-    <row r="38" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="84" t="s">
+      <c r="F37" s="57"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="65"/>
+    </row>
+    <row r="38" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="48" t="s">
+      <c r="D38" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E38" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="45"/>
-      <c r="G38" s="48" t="s">
+      <c r="F38" s="57"/>
+      <c r="G38" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="78" t="s">
+      <c r="H38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="74" t="s">
+      <c r="I38" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="J38" s="51"/>
-      <c r="K38" s="53" t="s">
+      <c r="J38" s="49"/>
+      <c r="K38" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="L38" s="36"/>
-      <c r="M38" s="49"/>
-    </row>
-    <row r="39" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
-      <c r="A39" s="85"/>
-      <c r="B39" s="50" t="s">
+      <c r="L38" s="22"/>
+      <c r="M38" s="52"/>
+    </row>
+    <row r="39" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="66"/>
+      <c r="B39" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="51"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="39" t="s">
+      <c r="C39" s="49"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="54"/>
-    </row>
-    <row r="40" spans="1:13" ht="61.5" thickTop="1" thickBot="1">
-      <c r="A40" s="85"/>
-      <c r="B40" s="22" t="s">
+      <c r="F39" s="57"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="64"/>
+    </row>
+    <row r="40" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="66"/>
+      <c r="B40" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="39" t="s">
+      <c r="C40" s="49"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="F40" s="45"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="54"/>
-    </row>
-    <row r="41" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A41" s="85"/>
-      <c r="B41" s="22" t="s">
+      <c r="F40" s="57"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="64"/>
+    </row>
+    <row r="41" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="66"/>
+      <c r="B41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="39" t="s">
+      <c r="C41" s="49"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="45"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="54"/>
-    </row>
-    <row r="42" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A42" s="86"/>
-      <c r="B42" s="22" t="s">
+      <c r="F41" s="57"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="64"/>
+    </row>
+    <row r="42" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="72"/>
+      <c r="B42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="55"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="39" t="s">
+      <c r="C42" s="68"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="57"/>
-    </row>
-    <row r="43" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A43" s="21" t="s">
+      <c r="F42" s="57"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="68"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="65"/>
+    </row>
+    <row r="43" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="48" t="s">
+      <c r="D43" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="48" t="s">
+      <c r="E43" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="F43" s="45"/>
-      <c r="G43" s="48" t="s">
+      <c r="F43" s="57"/>
+      <c r="G43" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="H43" s="78" t="s">
+      <c r="H43" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="59"/>
-      <c r="J43" s="46" t="s">
+      <c r="I43" s="80"/>
+      <c r="J43" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="K43" s="48" t="s">
+      <c r="K43" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="L43" s="36"/>
-      <c r="M43" s="49"/>
-    </row>
-    <row r="44" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
-      <c r="A44" s="40"/>
-      <c r="B44" s="50" t="s">
+      <c r="L43" s="22"/>
+      <c r="M43" s="52"/>
+    </row>
+    <row r="44" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="84"/>
+      <c r="B44" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="63"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="57"/>
-    </row>
-    <row r="45" spans="1:13" ht="61.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A45" s="84" t="s">
+      <c r="C44" s="68"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="81"/>
+      <c r="J44" s="68"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="65"/>
+    </row>
+    <row r="45" spans="1:13" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="C45" s="51" t="s">
+      <c r="C45" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="D45" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="48" t="s">
+      <c r="E45" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="F45" s="45"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="78" t="s">
+      <c r="F45" s="57"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I45" s="53" t="s">
+      <c r="I45" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="J45" s="61"/>
-      <c r="K45" s="54" t="s">
+      <c r="J45" s="82"/>
+      <c r="K45" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="L45" s="36"/>
-      <c r="M45" s="49"/>
-    </row>
-    <row r="46" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A46" s="85"/>
-      <c r="B46" s="50" t="s">
+      <c r="L45" s="22"/>
+      <c r="M45" s="52"/>
+    </row>
+    <row r="46" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="66"/>
+      <c r="B46" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="54"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="54"/>
-    </row>
-    <row r="47" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A47" s="85"/>
-      <c r="B47" s="22" t="s">
+      <c r="C46" s="49"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="82"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="64"/>
+    </row>
+    <row r="47" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="66"/>
+      <c r="B47" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="54"/>
-    </row>
-    <row r="48" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A48" s="86"/>
-      <c r="B48" s="22" t="s">
+      <c r="C47" s="49"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="82"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="64"/>
+    </row>
+    <row r="48" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="72"/>
+      <c r="B48" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="51"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="54"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="57"/>
-    </row>
-    <row r="49" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A49" s="84" t="s">
+      <c r="C48" s="49"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="82"/>
+      <c r="K48" s="64"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="65"/>
+    </row>
+    <row r="49" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="77" t="s">
+      <c r="B49" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="48" t="s">
+      <c r="D49" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="48" t="s">
+      <c r="E49" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="F49" s="45"/>
-      <c r="G49" s="48" t="s">
+      <c r="F49" s="57"/>
+      <c r="G49" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="78" t="s">
+      <c r="H49" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I49" s="59"/>
-      <c r="J49" s="46" t="s">
+      <c r="I49" s="80"/>
+      <c r="J49" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="K49" s="49" t="s">
+      <c r="K49" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="L49" s="36"/>
-      <c r="M49" s="49"/>
-    </row>
-    <row r="50" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A50" s="86"/>
-      <c r="B50" s="81"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="63"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="57"/>
-    </row>
-    <row r="51" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A51" s="84" t="s">
+      <c r="L49" s="22"/>
+      <c r="M49" s="52"/>
+    </row>
+    <row r="50" spans="1:13" ht="104.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="72"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="81"/>
+      <c r="J50" s="68"/>
+      <c r="K50" s="65"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="65"/>
+    </row>
+    <row r="51" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="C51" s="51" t="s">
+      <c r="C51" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="53" t="s">
+      <c r="D51" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="E51" s="48" t="s">
+      <c r="E51" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="F51" s="45"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="78" t="s">
+      <c r="F51" s="57"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I51" s="53"/>
-      <c r="J51" s="53" t="s">
+      <c r="I51" s="44"/>
+      <c r="J51" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="K51" s="53" t="s">
+      <c r="K51" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="L51" s="36"/>
-      <c r="M51" s="49"/>
-    </row>
-    <row r="52" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A52" s="85"/>
-      <c r="B52" s="22" t="s">
+      <c r="L51" s="22"/>
+      <c r="M51" s="52"/>
+    </row>
+    <row r="52" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="66"/>
+      <c r="B52" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="51"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="53"/>
-      <c r="J52" s="53"/>
-      <c r="K52" s="53"/>
-      <c r="L52" s="36"/>
-      <c r="M52" s="54"/>
-    </row>
-    <row r="53" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A53" s="86"/>
-      <c r="B53" s="22" t="s">
+      <c r="C52" s="49"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="64"/>
+    </row>
+    <row r="53" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="72"/>
+      <c r="B53" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="55"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="63"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="63"/>
-      <c r="J53" s="63"/>
-      <c r="K53" s="63"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="57"/>
-    </row>
-    <row r="54" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A54" s="84" t="s">
+      <c r="C53" s="68"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="65"/>
+    </row>
+    <row r="54" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="48" t="s">
+      <c r="D54" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="E54" s="48" t="s">
+      <c r="E54" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="F54" s="45"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="78" t="s">
+      <c r="F54" s="57"/>
+      <c r="G54" s="56"/>
+      <c r="H54" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I54" s="48" t="s">
+      <c r="I54" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="J54" s="48"/>
-      <c r="K54" s="48" t="s">
+      <c r="J54" s="56"/>
+      <c r="K54" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="L54" s="36"/>
-      <c r="M54" s="49"/>
-    </row>
-    <row r="55" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
-      <c r="A55" s="85"/>
-      <c r="B55" s="50" t="s">
+      <c r="L54" s="22"/>
+      <c r="M54" s="52"/>
+    </row>
+    <row r="55" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="66"/>
+      <c r="B55" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="51"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="53"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="53"/>
-      <c r="J55" s="53"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="54"/>
-    </row>
-    <row r="56" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A56" s="85"/>
-      <c r="B56" s="22" t="s">
+      <c r="C55" s="49"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="57"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="44"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="64"/>
+    </row>
+    <row r="56" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="66"/>
+      <c r="B56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C56" s="51"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="53"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="36"/>
-      <c r="M56" s="54"/>
-    </row>
-    <row r="57" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A57" s="86"/>
-      <c r="B57" s="22" t="s">
+      <c r="C56" s="49"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="57"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="64"/>
+    </row>
+    <row r="57" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="72"/>
+      <c r="B57" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="55"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="63"/>
-      <c r="J57" s="63"/>
-      <c r="K57" s="63"/>
-      <c r="L57" s="36"/>
-      <c r="M57" s="57"/>
-    </row>
-    <row r="58" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A58" s="84" t="s">
+      <c r="C57" s="68"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="57"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="57"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="62"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="65"/>
+    </row>
+    <row r="58" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B58" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="46" t="s">
+      <c r="C58" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="48" t="s">
+      <c r="D58" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="E58" s="48" t="s">
+      <c r="E58" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="F58" s="45"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="78" t="s">
+      <c r="F58" s="57"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I58" s="72" t="s">
+      <c r="I58" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="J58" s="87"/>
-      <c r="K58" s="48" t="s">
+      <c r="J58" s="34"/>
+      <c r="K58" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="L58" s="36"/>
-      <c r="M58" s="49"/>
-    </row>
-    <row r="59" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
-      <c r="A59" s="85"/>
-      <c r="B59" s="50" t="s">
+      <c r="L58" s="22"/>
+      <c r="M58" s="52"/>
+    </row>
+    <row r="59" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="66"/>
+      <c r="B59" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="51"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="53"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="74"/>
-      <c r="J59" s="88"/>
-      <c r="K59" s="53"/>
-      <c r="L59" s="36"/>
-      <c r="M59" s="54"/>
-    </row>
-    <row r="60" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A60" s="85"/>
-      <c r="B60" s="22" t="s">
+      <c r="C59" s="49"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="64"/>
+    </row>
+    <row r="60" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="66"/>
+      <c r="B60" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C60" s="51"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="53"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="74"/>
-      <c r="J60" s="88"/>
-      <c r="K60" s="53"/>
-      <c r="L60" s="36"/>
-      <c r="M60" s="54"/>
-    </row>
-    <row r="61" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A61" s="86"/>
-      <c r="B61" s="22" t="s">
+      <c r="C60" s="49"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="57"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="64"/>
+    </row>
+    <row r="61" spans="1:13" ht="107.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="72"/>
+      <c r="B61" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="55"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63"/>
-      <c r="F61" s="45"/>
-      <c r="G61" s="63"/>
-      <c r="H61" s="45"/>
-      <c r="I61" s="76"/>
-      <c r="J61" s="89"/>
-      <c r="K61" s="63"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="57"/>
-    </row>
-    <row r="62" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="84" t="s">
+      <c r="C61" s="68"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="74"/>
+      <c r="J61" s="36"/>
+      <c r="K61" s="62"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="65"/>
+    </row>
+    <row r="62" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="50" t="s">
+      <c r="B62" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C62" s="46" t="s">
+      <c r="C62" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D62" s="90" t="s">
+      <c r="D62" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="E62" s="48" t="s">
+      <c r="E62" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="F62" s="45"/>
-      <c r="G62" s="48" t="s">
+      <c r="F62" s="57"/>
+      <c r="G62" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="H62" s="78" t="s">
+      <c r="H62" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I62" s="72" t="s">
+      <c r="I62" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="J62" s="46"/>
-      <c r="K62" s="48" t="s">
+      <c r="J62" s="67"/>
+      <c r="K62" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="L62" s="36"/>
-      <c r="M62" s="49"/>
-    </row>
-    <row r="63" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A63" s="85"/>
-      <c r="B63" s="91" t="s">
+      <c r="L62" s="22"/>
+      <c r="M62" s="52"/>
+    </row>
+    <row r="63" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="66"/>
+      <c r="B63" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="51"/>
-      <c r="D63" s="92"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="45"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="74"/>
-      <c r="J63" s="51"/>
-      <c r="K63" s="53"/>
-      <c r="L63" s="36"/>
-      <c r="M63" s="54"/>
-    </row>
-    <row r="64" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A64" s="85"/>
-      <c r="B64" s="22" t="s">
+      <c r="C63" s="49"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="57"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="48"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="44"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="64"/>
+    </row>
+    <row r="64" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="66"/>
+      <c r="B64" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C64" s="51"/>
-      <c r="D64" s="92"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="53"/>
-      <c r="H64" s="45"/>
-      <c r="I64" s="74"/>
-      <c r="J64" s="51"/>
-      <c r="K64" s="53"/>
-      <c r="L64" s="36"/>
-      <c r="M64" s="54"/>
-    </row>
-    <row r="65" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A65" s="86"/>
-      <c r="B65" s="22" t="s">
+      <c r="C64" s="49"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="57"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="57"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="44"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="64"/>
+    </row>
+    <row r="65" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="72"/>
+      <c r="B65" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C65" s="55"/>
-      <c r="D65" s="93"/>
-      <c r="E65" s="63"/>
-      <c r="F65" s="45"/>
-      <c r="G65" s="63"/>
-      <c r="H65" s="45"/>
-      <c r="I65" s="76"/>
-      <c r="J65" s="55"/>
-      <c r="K65" s="63"/>
-      <c r="L65" s="36"/>
-      <c r="M65" s="57"/>
-    </row>
-    <row r="66" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A66" s="84" t="s">
+      <c r="C65" s="68"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="57"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="57"/>
+      <c r="I65" s="74"/>
+      <c r="J65" s="68"/>
+      <c r="K65" s="62"/>
+      <c r="L65" s="22"/>
+      <c r="M65" s="65"/>
+    </row>
+    <row r="66" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="B66" s="50" t="s">
+      <c r="B66" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C66" s="46" t="s">
+      <c r="C66" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="48" t="s">
+      <c r="D66" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="E66" s="48" t="s">
+      <c r="E66" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="F66" s="45"/>
-      <c r="G66" s="48" t="s">
+      <c r="F66" s="57"/>
+      <c r="G66" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="H66" s="78" t="s">
+      <c r="H66" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I66" s="72" t="s">
+      <c r="I66" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="J66" s="46"/>
-      <c r="K66" s="48" t="s">
+      <c r="J66" s="67"/>
+      <c r="K66" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="L66" s="36"/>
-      <c r="M66" s="49"/>
-    </row>
-    <row r="67" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A67" s="85"/>
-      <c r="B67" s="50" t="s">
+      <c r="L66" s="22"/>
+      <c r="M66" s="52"/>
+    </row>
+    <row r="67" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="66"/>
+      <c r="B67" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C67" s="51"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="45"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="45"/>
-      <c r="I67" s="74"/>
-      <c r="J67" s="51"/>
-      <c r="K67" s="53"/>
-      <c r="L67" s="36"/>
-      <c r="M67" s="54"/>
-    </row>
-    <row r="68" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A68" s="85"/>
-      <c r="B68" s="22" t="s">
+      <c r="C67" s="49"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="57"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="57"/>
+      <c r="I67" s="48"/>
+      <c r="J67" s="49"/>
+      <c r="K67" s="44"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="64"/>
+    </row>
+    <row r="68" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="66"/>
+      <c r="B68" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C68" s="51"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="45"/>
-      <c r="G68" s="53"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="74"/>
-      <c r="J68" s="51"/>
-      <c r="K68" s="53"/>
-      <c r="L68" s="36"/>
-      <c r="M68" s="54"/>
-    </row>
-    <row r="69" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A69" s="86"/>
-      <c r="B69" s="22" t="s">
+      <c r="C68" s="49"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="57"/>
+      <c r="G68" s="44"/>
+      <c r="H68" s="57"/>
+      <c r="I68" s="48"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="44"/>
+      <c r="L68" s="22"/>
+      <c r="M68" s="64"/>
+    </row>
+    <row r="69" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="72"/>
+      <c r="B69" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C69" s="55"/>
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="63"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="76"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="63"/>
-      <c r="L69" s="36"/>
-      <c r="M69" s="57"/>
-    </row>
-    <row r="70" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A70" s="84" t="s">
+      <c r="C69" s="68"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="57"/>
+      <c r="G69" s="62"/>
+      <c r="H69" s="57"/>
+      <c r="I69" s="74"/>
+      <c r="J69" s="68"/>
+      <c r="K69" s="62"/>
+      <c r="L69" s="22"/>
+      <c r="M69" s="65"/>
+    </row>
+    <row r="70" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="50" t="s">
+      <c r="B70" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="C70" s="46" t="s">
+      <c r="C70" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D70" s="48" t="s">
+      <c r="D70" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="E70" s="48" t="s">
+      <c r="E70" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="F70" s="45"/>
-      <c r="G70" s="48" t="s">
+      <c r="F70" s="57"/>
+      <c r="G70" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="H70" s="78" t="s">
+      <c r="H70" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I70" s="72" t="s">
+      <c r="I70" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="J70" s="46"/>
-      <c r="K70" s="48" t="s">
+      <c r="J70" s="67"/>
+      <c r="K70" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="L70" s="36"/>
-      <c r="M70" s="49"/>
-    </row>
-    <row r="71" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A71" s="85"/>
-      <c r="B71" s="50" t="s">
+      <c r="L70" s="22"/>
+      <c r="M70" s="52"/>
+    </row>
+    <row r="71" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="66"/>
+      <c r="B71" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="51"/>
-      <c r="D71" s="53"/>
-      <c r="E71" s="53"/>
-      <c r="F71" s="45"/>
-      <c r="G71" s="53"/>
-      <c r="H71" s="45"/>
-      <c r="I71" s="74"/>
-      <c r="J71" s="51"/>
-      <c r="K71" s="53"/>
-      <c r="L71" s="36"/>
-      <c r="M71" s="54"/>
-    </row>
-    <row r="72" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A72" s="85"/>
-      <c r="B72" s="22" t="s">
+      <c r="C71" s="49"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="57"/>
+      <c r="I71" s="48"/>
+      <c r="J71" s="49"/>
+      <c r="K71" s="44"/>
+      <c r="L71" s="22"/>
+      <c r="M71" s="64"/>
+    </row>
+    <row r="72" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="66"/>
+      <c r="B72" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C72" s="51"/>
-      <c r="D72" s="53"/>
-      <c r="E72" s="53"/>
-      <c r="F72" s="45"/>
-      <c r="G72" s="53"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="74"/>
-      <c r="J72" s="51"/>
-      <c r="K72" s="53"/>
-      <c r="L72" s="36"/>
-      <c r="M72" s="54"/>
-    </row>
-    <row r="73" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A73" s="86"/>
-      <c r="B73" s="22" t="s">
+      <c r="C72" s="49"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="57"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="57"/>
+      <c r="I72" s="48"/>
+      <c r="J72" s="49"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="22"/>
+      <c r="M72" s="64"/>
+    </row>
+    <row r="73" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="72"/>
+      <c r="B73" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C73" s="55"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="63"/>
-      <c r="F73" s="45"/>
-      <c r="G73" s="63"/>
-      <c r="H73" s="45"/>
-      <c r="I73" s="76"/>
-      <c r="J73" s="55"/>
-      <c r="K73" s="63"/>
-      <c r="L73" s="36"/>
-      <c r="M73" s="57"/>
-    </row>
-    <row r="74" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A74" s="84" t="s">
+      <c r="C73" s="68"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="57"/>
+      <c r="G73" s="62"/>
+      <c r="H73" s="57"/>
+      <c r="I73" s="74"/>
+      <c r="J73" s="68"/>
+      <c r="K73" s="62"/>
+      <c r="L73" s="22"/>
+      <c r="M73" s="65"/>
+    </row>
+    <row r="74" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="B74" s="50" t="s">
+      <c r="B74" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="C74" s="46" t="s">
+      <c r="C74" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D74" s="48" t="s">
+      <c r="D74" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E74" s="48" t="s">
+      <c r="E74" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="F74" s="45"/>
-      <c r="G74" s="48"/>
-      <c r="H74" s="78" t="s">
+      <c r="F74" s="57"/>
+      <c r="G74" s="56"/>
+      <c r="H74" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I74" s="48" t="s">
+      <c r="I74" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="J74" s="48"/>
-      <c r="K74" s="48" t="s">
+      <c r="J74" s="56"/>
+      <c r="K74" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="L74" s="36"/>
-      <c r="M74" s="49"/>
-    </row>
-    <row r="75" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A75" s="85"/>
-      <c r="B75" s="50" t="s">
+      <c r="L74" s="22"/>
+      <c r="M74" s="52"/>
+    </row>
+    <row r="75" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="66"/>
+      <c r="B75" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C75" s="51"/>
-      <c r="D75" s="53"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="53"/>
-      <c r="H75" s="45"/>
-      <c r="I75" s="53"/>
-      <c r="J75" s="53"/>
-      <c r="K75" s="53"/>
-      <c r="L75" s="36"/>
-      <c r="M75" s="54"/>
-    </row>
-    <row r="76" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A76" s="85"/>
-      <c r="B76" s="50" t="s">
+      <c r="C75" s="49"/>
+      <c r="D75" s="44"/>
+      <c r="E75" s="44"/>
+      <c r="F75" s="57"/>
+      <c r="G75" s="44"/>
+      <c r="H75" s="57"/>
+      <c r="I75" s="44"/>
+      <c r="J75" s="44"/>
+      <c r="K75" s="44"/>
+      <c r="L75" s="22"/>
+      <c r="M75" s="64"/>
+    </row>
+    <row r="76" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="66"/>
+      <c r="B76" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="C76" s="51"/>
-      <c r="D76" s="53"/>
-      <c r="E76" s="53"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="53"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="53"/>
-      <c r="J76" s="53"/>
-      <c r="K76" s="53"/>
-      <c r="L76" s="36"/>
-      <c r="M76" s="54"/>
-    </row>
-    <row r="77" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A77" s="85"/>
-      <c r="B77" s="22" t="s">
+      <c r="C76" s="49"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="57"/>
+      <c r="G76" s="44"/>
+      <c r="H76" s="57"/>
+      <c r="I76" s="44"/>
+      <c r="J76" s="44"/>
+      <c r="K76" s="44"/>
+      <c r="L76" s="22"/>
+      <c r="M76" s="64"/>
+    </row>
+    <row r="77" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="66"/>
+      <c r="B77" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C77" s="51"/>
-      <c r="D77" s="53"/>
-      <c r="E77" s="53"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="53"/>
-      <c r="H77" s="45"/>
-      <c r="I77" s="53"/>
-      <c r="J77" s="53"/>
-      <c r="K77" s="53"/>
-      <c r="L77" s="36"/>
-      <c r="M77" s="54"/>
-    </row>
-    <row r="78" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A78" s="86"/>
-      <c r="B78" s="22" t="s">
+      <c r="C77" s="49"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="57"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="57"/>
+      <c r="I77" s="44"/>
+      <c r="J77" s="44"/>
+      <c r="K77" s="44"/>
+      <c r="L77" s="22"/>
+      <c r="M77" s="64"/>
+    </row>
+    <row r="78" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="72"/>
+      <c r="B78" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="55"/>
-      <c r="D78" s="63"/>
-      <c r="E78" s="63"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="45"/>
-      <c r="I78" s="63"/>
-      <c r="J78" s="63"/>
-      <c r="K78" s="63"/>
-      <c r="L78" s="36"/>
-      <c r="M78" s="57"/>
-    </row>
-    <row r="79" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A79" s="84" t="s">
+      <c r="C78" s="68"/>
+      <c r="D78" s="62"/>
+      <c r="E78" s="62"/>
+      <c r="F78" s="57"/>
+      <c r="G78" s="62"/>
+      <c r="H78" s="57"/>
+      <c r="I78" s="62"/>
+      <c r="J78" s="62"/>
+      <c r="K78" s="62"/>
+      <c r="L78" s="22"/>
+      <c r="M78" s="65"/>
+    </row>
+    <row r="79" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="50" t="s">
+      <c r="B79" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="C79" s="46" t="s">
+      <c r="C79" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D79" s="48" t="s">
+      <c r="D79" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E79" s="48" t="s">
+      <c r="E79" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="F79" s="45"/>
-      <c r="G79" s="48"/>
-      <c r="H79" s="78" t="s">
+      <c r="F79" s="57"/>
+      <c r="G79" s="56"/>
+      <c r="H79" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I79" s="48" t="s">
+      <c r="I79" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="J79" s="48"/>
-      <c r="K79" s="48" t="s">
+      <c r="J79" s="56"/>
+      <c r="K79" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="L79" s="36"/>
-      <c r="M79" s="49"/>
-    </row>
-    <row r="80" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A80" s="85"/>
-      <c r="B80" s="50" t="s">
+      <c r="L79" s="22"/>
+      <c r="M79" s="52"/>
+    </row>
+    <row r="80" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="66"/>
+      <c r="B80" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C80" s="51"/>
-      <c r="D80" s="53"/>
-      <c r="E80" s="53"/>
-      <c r="F80" s="45"/>
-      <c r="G80" s="53"/>
-      <c r="H80" s="45"/>
-      <c r="I80" s="53"/>
-      <c r="J80" s="53"/>
-      <c r="K80" s="53"/>
-      <c r="L80" s="36"/>
-      <c r="M80" s="54"/>
-    </row>
-    <row r="81" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A81" s="85"/>
-      <c r="B81" s="50" t="s">
+      <c r="C80" s="49"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="57"/>
+      <c r="I80" s="44"/>
+      <c r="J80" s="44"/>
+      <c r="K80" s="44"/>
+      <c r="L80" s="22"/>
+      <c r="M80" s="64"/>
+    </row>
+    <row r="81" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="66"/>
+      <c r="B81" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="C81" s="51"/>
-      <c r="D81" s="53"/>
-      <c r="E81" s="53"/>
-      <c r="F81" s="45"/>
-      <c r="G81" s="53"/>
-      <c r="H81" s="45"/>
-      <c r="I81" s="53"/>
-      <c r="J81" s="53"/>
-      <c r="K81" s="53"/>
-      <c r="L81" s="36"/>
-      <c r="M81" s="54"/>
-    </row>
-    <row r="82" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A82" s="85"/>
-      <c r="B82" s="22" t="s">
+      <c r="C81" s="49"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="57"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="57"/>
+      <c r="I81" s="44"/>
+      <c r="J81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="22"/>
+      <c r="M81" s="64"/>
+    </row>
+    <row r="82" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="66"/>
+      <c r="B82" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C82" s="51"/>
-      <c r="D82" s="53"/>
-      <c r="E82" s="53"/>
-      <c r="F82" s="45"/>
-      <c r="G82" s="53"/>
-      <c r="H82" s="45"/>
-      <c r="I82" s="53"/>
-      <c r="J82" s="53"/>
-      <c r="K82" s="53"/>
-      <c r="L82" s="36"/>
-      <c r="M82" s="54"/>
-    </row>
-    <row r="83" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A83" s="86"/>
-      <c r="B83" s="22" t="s">
+      <c r="C82" s="49"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="57"/>
+      <c r="G82" s="44"/>
+      <c r="H82" s="57"/>
+      <c r="I82" s="44"/>
+      <c r="J82" s="44"/>
+      <c r="K82" s="44"/>
+      <c r="L82" s="22"/>
+      <c r="M82" s="64"/>
+    </row>
+    <row r="83" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="72"/>
+      <c r="B83" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C83" s="55"/>
-      <c r="D83" s="63"/>
-      <c r="E83" s="63"/>
-      <c r="F83" s="45"/>
-      <c r="G83" s="63"/>
-      <c r="H83" s="45"/>
-      <c r="I83" s="63"/>
-      <c r="J83" s="63"/>
-      <c r="K83" s="63"/>
-      <c r="L83" s="36"/>
-      <c r="M83" s="57"/>
-    </row>
-    <row r="84" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A84" s="84" t="s">
+      <c r="C83" s="68"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="62"/>
+      <c r="F83" s="57"/>
+      <c r="G83" s="62"/>
+      <c r="H83" s="57"/>
+      <c r="I83" s="62"/>
+      <c r="J83" s="62"/>
+      <c r="K83" s="62"/>
+      <c r="L83" s="22"/>
+      <c r="M83" s="65"/>
+    </row>
+    <row r="84" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="B84" s="50" t="s">
+      <c r="B84" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="C84" s="46" t="s">
+      <c r="C84" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D84" s="48" t="s">
+      <c r="D84" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="E84" s="48" t="s">
+      <c r="E84" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="F84" s="45"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="78" t="s">
+      <c r="F84" s="57"/>
+      <c r="G84" s="56"/>
+      <c r="H84" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I84" s="48" t="s">
+      <c r="I84" s="56" t="s">
         <v>170</v>
       </c>
-      <c r="J84" s="48"/>
-      <c r="K84" s="48" t="s">
+      <c r="J84" s="56"/>
+      <c r="K84" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="L84" s="36"/>
-      <c r="M84" s="49"/>
-    </row>
-    <row r="85" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A85" s="85"/>
-      <c r="B85" s="50" t="s">
+      <c r="L84" s="22"/>
+      <c r="M84" s="52"/>
+    </row>
+    <row r="85" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="66"/>
+      <c r="B85" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="C85" s="51"/>
-      <c r="D85" s="53"/>
-      <c r="E85" s="53"/>
-      <c r="F85" s="45"/>
-      <c r="G85" s="53"/>
-      <c r="H85" s="45"/>
-      <c r="I85" s="53"/>
-      <c r="J85" s="53"/>
-      <c r="K85" s="53"/>
-      <c r="L85" s="36"/>
-      <c r="M85" s="54"/>
-    </row>
-    <row r="86" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A86" s="85"/>
-      <c r="B86" s="22" t="s">
+      <c r="C85" s="49"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="57"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="57"/>
+      <c r="I85" s="44"/>
+      <c r="J85" s="44"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="22"/>
+      <c r="M85" s="64"/>
+    </row>
+    <row r="86" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="66"/>
+      <c r="B86" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C86" s="51"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="45"/>
-      <c r="G86" s="53"/>
-      <c r="H86" s="45"/>
-      <c r="I86" s="53"/>
-      <c r="J86" s="53"/>
-      <c r="K86" s="53"/>
-      <c r="L86" s="36"/>
-      <c r="M86" s="54"/>
-    </row>
-    <row r="87" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A87" s="94"/>
-      <c r="B87" s="22" t="s">
+      <c r="C86" s="49"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="57"/>
+      <c r="G86" s="44"/>
+      <c r="H86" s="57"/>
+      <c r="I86" s="44"/>
+      <c r="J86" s="44"/>
+      <c r="K86" s="44"/>
+      <c r="L86" s="22"/>
+      <c r="M86" s="64"/>
+    </row>
+    <row r="87" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="55"/>
+      <c r="B87" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C87" s="55"/>
-      <c r="D87" s="63"/>
-      <c r="E87" s="63"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="63"/>
-      <c r="H87" s="45"/>
-      <c r="I87" s="63"/>
-      <c r="J87" s="63"/>
-      <c r="K87" s="63"/>
-      <c r="L87" s="36"/>
-      <c r="M87" s="57"/>
-    </row>
-    <row r="88" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
-      <c r="A88" s="95" t="s">
+      <c r="C87" s="68"/>
+      <c r="D87" s="62"/>
+      <c r="E87" s="62"/>
+      <c r="F87" s="57"/>
+      <c r="G87" s="62"/>
+      <c r="H87" s="57"/>
+      <c r="I87" s="62"/>
+      <c r="J87" s="62"/>
+      <c r="K87" s="62"/>
+      <c r="L87" s="22"/>
+      <c r="M87" s="65"/>
+    </row>
+    <row r="88" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="22" t="s">
+      <c r="B88" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C88" s="46" t="s">
+      <c r="C88" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="D88" s="48" t="s">
+      <c r="D88" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="E88" s="48" t="s">
+      <c r="E88" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="F88" s="45"/>
-      <c r="G88" s="48"/>
-      <c r="H88" s="78" t="s">
+      <c r="F88" s="57"/>
+      <c r="G88" s="56"/>
+      <c r="H88" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I88" s="47"/>
-      <c r="J88" s="96"/>
-      <c r="K88" s="48" t="s">
+      <c r="I88" s="30"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="L88" s="36"/>
-      <c r="M88" s="49"/>
-    </row>
-    <row r="89" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
-      <c r="A89" s="85"/>
-      <c r="B89" s="22" t="s">
+      <c r="L88" s="22"/>
+      <c r="M88" s="52"/>
+    </row>
+    <row r="89" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="66"/>
+      <c r="B89" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="51"/>
-      <c r="D89" s="53"/>
-      <c r="E89" s="53"/>
-      <c r="F89" s="45"/>
-      <c r="G89" s="53"/>
-      <c r="H89" s="45"/>
-      <c r="I89" s="52"/>
-      <c r="J89" s="97"/>
-      <c r="K89" s="53"/>
-      <c r="L89" s="36"/>
-      <c r="M89" s="54"/>
-    </row>
-    <row r="90" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A90" s="98" t="s">
+      <c r="C89" s="49"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="57"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="57"/>
+      <c r="I89" s="32"/>
+      <c r="J89" s="39"/>
+      <c r="K89" s="44"/>
+      <c r="L89" s="22"/>
+      <c r="M89" s="64"/>
+    </row>
+    <row r="90" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="99" t="s">
+      <c r="B90" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="C90" s="51"/>
-      <c r="D90" s="53"/>
-      <c r="E90" s="53"/>
-      <c r="F90" s="45"/>
-      <c r="G90" s="53"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="100" t="s">
+      <c r="C90" s="49"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="57"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="57"/>
+      <c r="I90" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="J90" s="97"/>
-      <c r="K90" s="53"/>
-      <c r="L90" s="36"/>
-      <c r="M90" s="54"/>
-    </row>
-    <row r="91" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A91" s="101"/>
-      <c r="B91" s="99" t="s">
+      <c r="J90" s="39"/>
+      <c r="K90" s="44"/>
+      <c r="L90" s="22"/>
+      <c r="M90" s="64"/>
+    </row>
+    <row r="91" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="59"/>
+      <c r="B91" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="C91" s="51"/>
-      <c r="D91" s="53"/>
-      <c r="E91" s="53"/>
-      <c r="F91" s="45"/>
-      <c r="G91" s="53"/>
-      <c r="H91" s="45"/>
-      <c r="I91" s="102"/>
-      <c r="J91" s="97"/>
-      <c r="K91" s="53"/>
-      <c r="L91" s="36"/>
-      <c r="M91" s="54"/>
-    </row>
-    <row r="92" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A92" s="98" t="s">
+      <c r="C91" s="49"/>
+      <c r="D91" s="44"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="57"/>
+      <c r="G91" s="44"/>
+      <c r="H91" s="57"/>
+      <c r="I91" s="61"/>
+      <c r="J91" s="39"/>
+      <c r="K91" s="44"/>
+      <c r="L91" s="22"/>
+      <c r="M91" s="64"/>
+    </row>
+    <row r="92" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="B92" s="50" t="s">
+      <c r="B92" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="C92" s="51"/>
-      <c r="D92" s="53"/>
-      <c r="E92" s="53"/>
-      <c r="F92" s="45"/>
-      <c r="G92" s="53"/>
-      <c r="H92" s="45"/>
-      <c r="I92" s="100" t="s">
+      <c r="C92" s="49"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="57"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="57"/>
+      <c r="I92" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="J92" s="97"/>
-      <c r="K92" s="53"/>
-      <c r="L92" s="36"/>
-      <c r="M92" s="54"/>
-    </row>
-    <row r="93" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A93" s="101"/>
-      <c r="B93" s="50" t="s">
+      <c r="J92" s="39"/>
+      <c r="K92" s="44"/>
+      <c r="L92" s="22"/>
+      <c r="M92" s="64"/>
+    </row>
+    <row r="93" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="59"/>
+      <c r="B93" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C93" s="51"/>
-      <c r="D93" s="53"/>
-      <c r="E93" s="53"/>
-      <c r="F93" s="45"/>
-      <c r="G93" s="53"/>
-      <c r="H93" s="45"/>
-      <c r="I93" s="102"/>
-      <c r="J93" s="97"/>
-      <c r="K93" s="53"/>
-      <c r="L93" s="36"/>
-      <c r="M93" s="54"/>
-    </row>
-    <row r="94" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A94" s="98" t="s">
+      <c r="C93" s="49"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="57"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="57"/>
+      <c r="I93" s="61"/>
+      <c r="J93" s="39"/>
+      <c r="K93" s="44"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="64"/>
+    </row>
+    <row r="94" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="B94" s="50" t="s">
+      <c r="B94" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="C94" s="51"/>
-      <c r="D94" s="53"/>
-      <c r="E94" s="53"/>
-      <c r="F94" s="45"/>
-      <c r="G94" s="53"/>
-      <c r="H94" s="45"/>
-      <c r="I94" s="103" t="s">
+      <c r="C94" s="49"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="57"/>
+      <c r="G94" s="44"/>
+      <c r="H94" s="57"/>
+      <c r="I94" s="69" t="s">
         <v>185</v>
       </c>
-      <c r="J94" s="97"/>
-      <c r="K94" s="53"/>
-      <c r="L94" s="36"/>
-      <c r="M94" s="54"/>
-    </row>
-    <row r="95" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A95" s="101"/>
-      <c r="B95" s="50" t="s">
+      <c r="J94" s="39"/>
+      <c r="K94" s="44"/>
+      <c r="L94" s="22"/>
+      <c r="M94" s="64"/>
+    </row>
+    <row r="95" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="59"/>
+      <c r="B95" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C95" s="51"/>
-      <c r="D95" s="53"/>
-      <c r="E95" s="53"/>
-      <c r="F95" s="45"/>
-      <c r="G95" s="53"/>
-      <c r="H95" s="45"/>
-      <c r="I95" s="104"/>
-      <c r="J95" s="97"/>
-      <c r="K95" s="53"/>
-      <c r="L95" s="36"/>
-      <c r="M95" s="54"/>
-    </row>
-    <row r="96" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A96" s="98" t="s">
+      <c r="C95" s="49"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="57"/>
+      <c r="G95" s="44"/>
+      <c r="H95" s="57"/>
+      <c r="I95" s="70"/>
+      <c r="J95" s="39"/>
+      <c r="K95" s="44"/>
+      <c r="L95" s="22"/>
+      <c r="M95" s="64"/>
+    </row>
+    <row r="96" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="B96" s="50" t="s">
+      <c r="B96" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="C96" s="51"/>
-      <c r="D96" s="53"/>
-      <c r="E96" s="53"/>
-      <c r="F96" s="45"/>
-      <c r="G96" s="53"/>
-      <c r="H96" s="45"/>
-      <c r="I96" s="100" t="s">
+      <c r="C96" s="49"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="44"/>
+      <c r="F96" s="57"/>
+      <c r="G96" s="44"/>
+      <c r="H96" s="57"/>
+      <c r="I96" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="J96" s="97"/>
-      <c r="K96" s="53"/>
-      <c r="L96" s="36"/>
-      <c r="M96" s="54"/>
-    </row>
-    <row r="97" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A97" s="101"/>
-      <c r="B97" s="50" t="s">
+      <c r="J96" s="39"/>
+      <c r="K96" s="44"/>
+      <c r="L96" s="22"/>
+      <c r="M96" s="64"/>
+    </row>
+    <row r="97" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="59"/>
+      <c r="B97" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C97" s="51"/>
-      <c r="D97" s="53"/>
-      <c r="E97" s="53"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="53"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="102"/>
-      <c r="J97" s="97"/>
-      <c r="K97" s="53"/>
-      <c r="L97" s="36"/>
-      <c r="M97" s="54"/>
-    </row>
-    <row r="98" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A98" s="98" t="s">
+      <c r="C97" s="49"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="57"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="57"/>
+      <c r="I97" s="61"/>
+      <c r="J97" s="39"/>
+      <c r="K97" s="44"/>
+      <c r="L97" s="22"/>
+      <c r="M97" s="64"/>
+    </row>
+    <row r="98" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="58" t="s">
         <v>189</v>
       </c>
-      <c r="B98" s="50" t="s">
+      <c r="B98" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="C98" s="51"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="53"/>
-      <c r="F98" s="45"/>
-      <c r="G98" s="53"/>
-      <c r="H98" s="45"/>
-      <c r="I98" s="100" t="s">
+      <c r="C98" s="49"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="57"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="57"/>
+      <c r="I98" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="J98" s="97"/>
-      <c r="K98" s="53"/>
-      <c r="L98" s="36"/>
-      <c r="M98" s="54"/>
-    </row>
-    <row r="99" spans="1:13" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A99" s="101"/>
-      <c r="B99" s="50" t="s">
+      <c r="J98" s="39"/>
+      <c r="K98" s="44"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="64"/>
+    </row>
+    <row r="99" spans="1:13" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="59"/>
+      <c r="B99" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C99" s="51"/>
-      <c r="D99" s="53"/>
-      <c r="E99" s="53"/>
-      <c r="F99" s="45"/>
-      <c r="G99" s="53"/>
-      <c r="H99" s="45"/>
-      <c r="I99" s="102"/>
-      <c r="J99" s="97"/>
-      <c r="K99" s="53"/>
-      <c r="L99" s="36"/>
-      <c r="M99" s="54"/>
-    </row>
-    <row r="100" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A100" s="98" t="s">
+      <c r="C99" s="49"/>
+      <c r="D99" s="44"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="57"/>
+      <c r="G99" s="44"/>
+      <c r="H99" s="57"/>
+      <c r="I99" s="61"/>
+      <c r="J99" s="39"/>
+      <c r="K99" s="44"/>
+      <c r="L99" s="22"/>
+      <c r="M99" s="64"/>
+    </row>
+    <row r="100" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="B100" s="50" t="s">
+      <c r="B100" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="C100" s="51"/>
-      <c r="D100" s="53"/>
-      <c r="E100" s="53"/>
-      <c r="F100" s="45"/>
-      <c r="G100" s="53"/>
-      <c r="H100" s="45"/>
-      <c r="I100" s="100" t="s">
+      <c r="C100" s="49"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="57"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="57"/>
+      <c r="I100" s="60" t="s">
         <v>194</v>
       </c>
-      <c r="J100" s="97"/>
-      <c r="K100" s="53"/>
-      <c r="L100" s="36"/>
-      <c r="M100" s="54"/>
-    </row>
-    <row r="101" spans="1:13" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A101" s="101"/>
-      <c r="B101" s="50" t="s">
+      <c r="J100" s="39"/>
+      <c r="K100" s="44"/>
+      <c r="L100" s="22"/>
+      <c r="M100" s="64"/>
+    </row>
+    <row r="101" spans="1:13" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="59"/>
+      <c r="B101" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C101" s="51"/>
-      <c r="D101" s="53"/>
-      <c r="E101" s="53"/>
-      <c r="F101" s="45"/>
-      <c r="G101" s="53"/>
-      <c r="H101" s="45"/>
-      <c r="I101" s="105"/>
-      <c r="J101" s="97"/>
-      <c r="K101" s="53"/>
-      <c r="L101" s="36"/>
-      <c r="M101" s="54"/>
-    </row>
-    <row r="102" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A102" s="98" t="s">
+      <c r="C101" s="49"/>
+      <c r="D101" s="44"/>
+      <c r="E101" s="44"/>
+      <c r="F101" s="57"/>
+      <c r="G101" s="44"/>
+      <c r="H101" s="57"/>
+      <c r="I101" s="63"/>
+      <c r="J101" s="39"/>
+      <c r="K101" s="44"/>
+      <c r="L101" s="22"/>
+      <c r="M101" s="64"/>
+    </row>
+    <row r="102" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="B102" s="50" t="s">
+      <c r="B102" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="C102" s="51"/>
-      <c r="D102" s="53"/>
-      <c r="E102" s="53"/>
-      <c r="F102" s="45"/>
-      <c r="G102" s="53"/>
-      <c r="H102" s="45"/>
-      <c r="I102" s="100" t="s">
+      <c r="C102" s="49"/>
+      <c r="D102" s="44"/>
+      <c r="E102" s="44"/>
+      <c r="F102" s="57"/>
+      <c r="G102" s="44"/>
+      <c r="H102" s="57"/>
+      <c r="I102" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="J102" s="97"/>
-      <c r="K102" s="53"/>
-      <c r="L102" s="36"/>
-      <c r="M102" s="54"/>
-    </row>
-    <row r="103" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A103" s="101"/>
-      <c r="B103" s="50" t="s">
+      <c r="J102" s="39"/>
+      <c r="K102" s="44"/>
+      <c r="L102" s="22"/>
+      <c r="M102" s="64"/>
+    </row>
+    <row r="103" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="59"/>
+      <c r="B103" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="C103" s="51"/>
-      <c r="D103" s="53"/>
-      <c r="E103" s="53"/>
-      <c r="F103" s="45"/>
-      <c r="G103" s="53"/>
-      <c r="H103" s="45"/>
-      <c r="I103" s="102"/>
-      <c r="J103" s="97"/>
-      <c r="K103" s="53"/>
-      <c r="L103" s="36"/>
-      <c r="M103" s="54"/>
-    </row>
-    <row r="104" spans="1:13" ht="28.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A104" s="98" t="s">
+      <c r="C103" s="49"/>
+      <c r="D103" s="44"/>
+      <c r="E103" s="44"/>
+      <c r="F103" s="57"/>
+      <c r="G103" s="44"/>
+      <c r="H103" s="57"/>
+      <c r="I103" s="61"/>
+      <c r="J103" s="39"/>
+      <c r="K103" s="44"/>
+      <c r="L103" s="22"/>
+      <c r="M103" s="64"/>
+    </row>
+    <row r="104" spans="1:13" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="B104" s="50" t="s">
+      <c r="B104" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="C104" s="51"/>
-      <c r="D104" s="53"/>
-      <c r="E104" s="53"/>
-      <c r="F104" s="45"/>
-      <c r="G104" s="53"/>
-      <c r="H104" s="45"/>
-      <c r="I104" s="100" t="s">
+      <c r="C104" s="49"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="44"/>
+      <c r="F104" s="57"/>
+      <c r="G104" s="44"/>
+      <c r="H104" s="57"/>
+      <c r="I104" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="J104" s="97"/>
-      <c r="K104" s="53"/>
-      <c r="L104" s="36"/>
-      <c r="M104" s="54"/>
-    </row>
-    <row r="105" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A105" s="101"/>
-      <c r="B105" s="50" t="s">
+      <c r="J104" s="39"/>
+      <c r="K104" s="44"/>
+      <c r="L104" s="22"/>
+      <c r="M104" s="64"/>
+    </row>
+    <row r="105" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="59"/>
+      <c r="B105" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="C105" s="51"/>
-      <c r="D105" s="53"/>
-      <c r="E105" s="53"/>
-      <c r="F105" s="45"/>
-      <c r="G105" s="53"/>
-      <c r="H105" s="45"/>
-      <c r="I105" s="102"/>
-      <c r="J105" s="97"/>
-      <c r="K105" s="53"/>
-      <c r="L105" s="36"/>
-      <c r="M105" s="54"/>
-    </row>
-    <row r="106" spans="1:13" ht="27.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A106" s="98" t="s">
+      <c r="C105" s="49"/>
+      <c r="D105" s="44"/>
+      <c r="E105" s="44"/>
+      <c r="F105" s="57"/>
+      <c r="G105" s="44"/>
+      <c r="H105" s="57"/>
+      <c r="I105" s="61"/>
+      <c r="J105" s="39"/>
+      <c r="K105" s="44"/>
+      <c r="L105" s="22"/>
+      <c r="M105" s="64"/>
+    </row>
+    <row r="106" spans="1:13" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="B106" s="50" t="s">
+      <c r="B106" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C106" s="51"/>
-      <c r="D106" s="53"/>
-      <c r="E106" s="53"/>
-      <c r="F106" s="45"/>
-      <c r="G106" s="53"/>
-      <c r="H106" s="45"/>
-      <c r="I106" s="100" t="s">
+      <c r="C106" s="49"/>
+      <c r="D106" s="44"/>
+      <c r="E106" s="44"/>
+      <c r="F106" s="57"/>
+      <c r="G106" s="44"/>
+      <c r="H106" s="57"/>
+      <c r="I106" s="60" t="s">
         <v>205</v>
       </c>
-      <c r="J106" s="97"/>
-      <c r="K106" s="53"/>
-      <c r="L106" s="36"/>
-      <c r="M106" s="54"/>
-    </row>
-    <row r="107" spans="1:13" ht="18" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A107" s="101"/>
-      <c r="B107" s="50" t="s">
+      <c r="J106" s="39"/>
+      <c r="K106" s="44"/>
+      <c r="L106" s="22"/>
+      <c r="M106" s="64"/>
+    </row>
+    <row r="107" spans="1:13" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="59"/>
+      <c r="B107" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="C107" s="55"/>
-      <c r="D107" s="63"/>
-      <c r="E107" s="63"/>
-      <c r="F107" s="45"/>
-      <c r="G107" s="63"/>
-      <c r="H107" s="45"/>
-      <c r="I107" s="63"/>
-      <c r="J107" s="106"/>
-      <c r="K107" s="63"/>
-      <c r="L107" s="36"/>
-      <c r="M107" s="57"/>
-    </row>
-    <row r="108" spans="1:13" ht="22.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A108" s="95" t="s">
+      <c r="C107" s="68"/>
+      <c r="D107" s="62"/>
+      <c r="E107" s="62"/>
+      <c r="F107" s="57"/>
+      <c r="G107" s="62"/>
+      <c r="H107" s="57"/>
+      <c r="I107" s="62"/>
+      <c r="J107" s="41"/>
+      <c r="K107" s="62"/>
+      <c r="L107" s="22"/>
+      <c r="M107" s="65"/>
+    </row>
+    <row r="108" spans="1:13" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="B108" s="50" t="s">
+      <c r="B108" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="C108" s="51" t="s">
+      <c r="C108" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D108" s="53" t="s">
+      <c r="D108" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="E108" s="48" t="s">
+      <c r="E108" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="F108" s="45"/>
-      <c r="G108" s="53" t="s">
+      <c r="F108" s="57"/>
+      <c r="G108" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="H108" s="78" t="s">
+      <c r="H108" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="I108" s="74" t="s">
+      <c r="I108" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="J108" s="51"/>
-      <c r="K108" s="53" t="s">
+      <c r="J108" s="49"/>
+      <c r="K108" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="L108" s="36"/>
-      <c r="M108" s="49"/>
-    </row>
-    <row r="109" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A109" s="94"/>
-      <c r="B109" s="107" t="s">
+      <c r="L108" s="22"/>
+      <c r="M108" s="52"/>
+    </row>
+    <row r="109" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="55"/>
+      <c r="B109" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="C109" s="108"/>
-      <c r="D109" s="109"/>
-      <c r="E109" s="109"/>
-      <c r="F109" s="110"/>
-      <c r="G109" s="109"/>
-      <c r="H109" s="110"/>
-      <c r="I109" s="111"/>
-      <c r="J109" s="108"/>
-      <c r="K109" s="109"/>
-      <c r="L109" s="112"/>
-      <c r="M109" s="113"/>
+      <c r="C109" s="51"/>
+      <c r="D109" s="45"/>
+      <c r="E109" s="45"/>
+      <c r="F109" s="47"/>
+      <c r="G109" s="45"/>
+      <c r="H109" s="47"/>
+      <c r="I109" s="50"/>
+      <c r="J109" s="51"/>
+      <c r="K109" s="45"/>
+      <c r="L109" s="43"/>
+      <c r="M109" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="251">
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="H108:H109"/>
-    <mergeCell ref="I108:J109"/>
-    <mergeCell ref="K108:K109"/>
-    <mergeCell ref="M108:M109"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="I102:I103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="I96:I97"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="I98:I99"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="K11:K14"/>
+    <mergeCell ref="M11:M14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="I15:I19"/>
+    <mergeCell ref="J15:J19"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="M15:M19"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="M20:M23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="I24:J27"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="M24:M27"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="G30:G34"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="I30:I34"/>
+    <mergeCell ref="J30:J34"/>
+    <mergeCell ref="K30:K34"/>
+    <mergeCell ref="M30:M33"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="K35:K37"/>
+    <mergeCell ref="M35:M37"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H38:H42"/>
+    <mergeCell ref="I38:J42"/>
+    <mergeCell ref="K38:K42"/>
+    <mergeCell ref="M38:M42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="F38:F42"/>
+    <mergeCell ref="G38:G42"/>
+    <mergeCell ref="M45:M48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="K49:K50"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="G45:G48"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="I45:I48"/>
+    <mergeCell ref="J45:J48"/>
+    <mergeCell ref="K45:K48"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="M51:M53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="I54:I57"/>
+    <mergeCell ref="J54:J57"/>
+    <mergeCell ref="K54:K57"/>
+    <mergeCell ref="M54:M57"/>
+    <mergeCell ref="G51:G53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="K51:K53"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="I58:I61"/>
+    <mergeCell ref="K58:K61"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="H62:H65"/>
+    <mergeCell ref="I62:J65"/>
+    <mergeCell ref="K62:K65"/>
+    <mergeCell ref="M62:M65"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="I66:J69"/>
+    <mergeCell ref="K66:K69"/>
+    <mergeCell ref="M66:M69"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:J73"/>
+    <mergeCell ref="K70:K73"/>
+    <mergeCell ref="M70:M73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="M74:M78"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="C79:C83"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="E79:E83"/>
+    <mergeCell ref="F79:F83"/>
+    <mergeCell ref="G79:G83"/>
+    <mergeCell ref="H79:H83"/>
+    <mergeCell ref="I79:I83"/>
+    <mergeCell ref="J79:J83"/>
+    <mergeCell ref="K79:K83"/>
+    <mergeCell ref="M79:M83"/>
+    <mergeCell ref="G74:G78"/>
+    <mergeCell ref="H74:H78"/>
+    <mergeCell ref="I74:I78"/>
+    <mergeCell ref="J74:J78"/>
+    <mergeCell ref="K74:K78"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="E74:E78"/>
+    <mergeCell ref="F74:F78"/>
     <mergeCell ref="M84:M87"/>
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="C88:C107"/>
@@ -6190,211 +6375,28 @@
     <mergeCell ref="A84:A87"/>
     <mergeCell ref="C84:C87"/>
     <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F84:F87"/>
-    <mergeCell ref="M74:M78"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="C79:C83"/>
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="E79:E83"/>
-    <mergeCell ref="F79:F83"/>
-    <mergeCell ref="G79:G83"/>
-    <mergeCell ref="H79:H83"/>
-    <mergeCell ref="I79:I83"/>
-    <mergeCell ref="J79:J83"/>
-    <mergeCell ref="K79:K83"/>
-    <mergeCell ref="M79:M83"/>
-    <mergeCell ref="G74:G78"/>
-    <mergeCell ref="H74:H78"/>
-    <mergeCell ref="I74:I78"/>
-    <mergeCell ref="J74:J78"/>
-    <mergeCell ref="K74:K78"/>
-    <mergeCell ref="A74:A78"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="E74:E78"/>
-    <mergeCell ref="F74:F78"/>
-    <mergeCell ref="G70:G73"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="I70:J73"/>
-    <mergeCell ref="K70:K73"/>
-    <mergeCell ref="M70:M73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="G66:G69"/>
-    <mergeCell ref="H66:H69"/>
-    <mergeCell ref="I66:J69"/>
-    <mergeCell ref="K66:K69"/>
-    <mergeCell ref="M66:M69"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="H62:H65"/>
-    <mergeCell ref="I62:J65"/>
-    <mergeCell ref="K62:K65"/>
-    <mergeCell ref="M62:M65"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="I58:I61"/>
-    <mergeCell ref="K58:K61"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="M51:M53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="G54:G57"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="I54:I57"/>
-    <mergeCell ref="J54:J57"/>
-    <mergeCell ref="K54:K57"/>
-    <mergeCell ref="M54:M57"/>
-    <mergeCell ref="G51:G53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="K51:K53"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="M45:M48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="K49:K50"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="G45:G48"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="I45:I48"/>
-    <mergeCell ref="J45:J48"/>
-    <mergeCell ref="K45:K48"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="H38:H42"/>
-    <mergeCell ref="I38:J42"/>
-    <mergeCell ref="K38:K42"/>
-    <mergeCell ref="M38:M42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="F38:F42"/>
-    <mergeCell ref="G38:G42"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="K35:K37"/>
-    <mergeCell ref="M35:M37"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="G30:G34"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="I30:I34"/>
-    <mergeCell ref="J30:J34"/>
-    <mergeCell ref="K30:K34"/>
-    <mergeCell ref="M30:M33"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="I24:J27"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="M24:M27"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="K11:K14"/>
-    <mergeCell ref="M11:M14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="J15:J19"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="M15:M19"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="I102:I103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="I96:I97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="H108:H109"/>
+    <mergeCell ref="I108:J109"/>
+    <mergeCell ref="K108:K109"/>
+    <mergeCell ref="M108:M109"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6404,24 +6406,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise a jour des fichier
</commit_message>
<xml_diff>
--- a/uploads/Conditions precedents to be satisfied on or before May 29, 2014.xlsx
+++ b/uploads/Conditions precedents to be satisfied on or before May 29, 2014.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="12240" windowHeight="7995"/>
@@ -2493,11 +2493,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3134,13 +3134,52 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3168,6 +3207,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3192,6 +3234,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3204,18 +3249,132 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3225,235 +3384,76 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3629,7 +3629,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3664,7 +3663,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3840,30 +3838,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
       <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="17" customWidth="1"/>
-    <col min="2" max="4" width="38.42578125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="20" style="17" customWidth="1"/>
-    <col min="6" max="6" width="52.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="18" style="17" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="17" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="17" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="17" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" style="17" customWidth="1"/>
-    <col min="13" max="13" width="29.28515625" style="17" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="13.42578125" style="30" customWidth="1"/>
+    <col min="2" max="4" width="38.42578125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="20" style="30" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="30" customWidth="1"/>
+    <col min="8" max="8" width="18" style="30" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="30" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="30" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="30" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" style="30" customWidth="1"/>
+    <col min="13" max="13" width="29.28515625" style="30" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3878,7 +3876,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="4" customFormat="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3893,2440 +3891,2305 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:13" s="6" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="104" t="s">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="77.25" customHeight="1" thickBot="1"/>
+    <row r="4" spans="1:13" s="12" customFormat="1" ht="33" customHeight="1" thickBot="1">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="111" t="s">
+      <c r="F4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="102" t="s">
+      <c r="G4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="108" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="113" t="s">
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="106"/>
-      <c r="K4" s="102" t="s">
+      <c r="J4" s="8"/>
+      <c r="K4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="102" t="s">
+      <c r="L4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="102" t="s">
+      <c r="M4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="105"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="7" t="s">
+    <row r="5" spans="1:13" s="12" customFormat="1" ht="18" customHeight="1" thickBot="1">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-    </row>
-    <row r="6" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="83" t="s">
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="25"/>
+      <c r="G6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13" t="s">
+      <c r="H6" s="25"/>
+      <c r="I6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="13" t="s">
+      <c r="J6" s="27"/>
+      <c r="K6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="16"/>
-    </row>
-    <row r="7" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101"/>
-      <c r="B7" s="9" t="s">
+      <c r="M6" s="29"/>
+    </row>
+    <row r="7" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="31"/>
+      <c r="B7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="23"/>
-    </row>
-    <row r="8" spans="1:13" ht="107.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="101"/>
-      <c r="B8" s="9" t="s">
+      <c r="F7" s="34"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+    </row>
+    <row r="8" spans="1:13" ht="107.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="31"/>
+      <c r="B8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="23"/>
-    </row>
-    <row r="9" spans="1:13" ht="52.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="101"/>
-      <c r="B9" s="9" t="s">
+      <c r="F8" s="34"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="1:13" ht="52.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="31"/>
+      <c r="B9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="10" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="84"/>
-      <c r="B10" s="9" t="s">
+      <c r="F9" s="38"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="37"/>
+    </row>
+    <row r="10" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A10" s="40"/>
+      <c r="B10" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="20" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="29"/>
-    </row>
-    <row r="11" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83" t="s">
+      <c r="F10" s="38"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="44"/>
+    </row>
+    <row r="11" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="67" t="s">
+      <c r="F11" s="34"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="56" t="s">
+      <c r="J11" s="47"/>
+      <c r="K11" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="52"/>
-    </row>
-    <row r="12" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101"/>
-      <c r="B12" s="31" t="s">
+      <c r="L11" s="36"/>
+      <c r="M11" s="49"/>
+    </row>
+    <row r="12" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
+      <c r="A12" s="31"/>
+      <c r="B12" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="20" t="s">
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="64"/>
-    </row>
-    <row r="13" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="101"/>
-      <c r="B13" s="9" t="s">
+      <c r="F12" s="38"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="54"/>
+    </row>
+    <row r="13" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A13" s="31"/>
+      <c r="B13" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="25" t="s">
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="64"/>
-    </row>
-    <row r="14" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="84"/>
-      <c r="B14" s="9" t="s">
+      <c r="F13" s="38"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="54"/>
+    </row>
+    <row r="14" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A14" s="40"/>
+      <c r="B14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="25" t="s">
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="65"/>
-    </row>
-    <row r="15" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="98" t="s">
+      <c r="F14" s="38"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="57"/>
+    </row>
+    <row r="15" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A15" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="56" t="s">
+      <c r="F15" s="39"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="80"/>
-      <c r="K15" s="56" t="s">
+      <c r="J15" s="59"/>
+      <c r="K15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="52"/>
-    </row>
-    <row r="16" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="99"/>
-      <c r="B16" s="9" t="s">
+      <c r="L15" s="36"/>
+      <c r="M15" s="49"/>
+    </row>
+    <row r="16" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A16" s="60"/>
+      <c r="B16" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="51"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="64"/>
-    </row>
-    <row r="17" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="99"/>
-      <c r="B17" s="31" t="s">
+      <c r="F16" s="39"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="54"/>
+    </row>
+    <row r="17" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
+      <c r="A17" s="60"/>
+      <c r="B17" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="25" t="s">
+      <c r="C17" s="51"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="64"/>
-    </row>
-    <row r="18" spans="1:13" ht="93" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="99"/>
-      <c r="B18" s="9" t="s">
+      <c r="F17" s="39"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="54"/>
+    </row>
+    <row r="18" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A18" s="60"/>
+      <c r="B18" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="51"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="64"/>
-    </row>
-    <row r="19" spans="1:13" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
-      <c r="B19" s="9" t="s">
+      <c r="F18" s="39"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="54"/>
+    </row>
+    <row r="19" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A19" s="62"/>
+      <c r="B19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="25" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="65"/>
-    </row>
-    <row r="20" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="92" t="s">
+      <c r="F19" s="39"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="57"/>
+    </row>
+    <row r="20" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A20" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="95" t="s">
+      <c r="D20" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="56" t="s">
+      <c r="F20" s="39"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="67" t="s">
+      <c r="J20" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="56" t="s">
+      <c r="K20" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="L20" s="22"/>
-      <c r="M20" s="52"/>
-    </row>
-    <row r="21" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="93"/>
-      <c r="B21" s="31" t="s">
+      <c r="L20" s="36"/>
+      <c r="M20" s="49"/>
+    </row>
+    <row r="21" spans="1:13" ht="61.5" thickTop="1" thickBot="1">
+      <c r="A21" s="67"/>
+      <c r="B21" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="64"/>
-    </row>
-    <row r="22" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="93"/>
-      <c r="B22" s="31" t="s">
+      <c r="C21" s="51"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="54"/>
+    </row>
+    <row r="22" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A22" s="67"/>
+      <c r="B22" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="64"/>
-    </row>
-    <row r="23" spans="1:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="94"/>
-      <c r="B23" s="31" t="s">
+      <c r="C22" s="51"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="54"/>
+    </row>
+    <row r="23" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
+      <c r="A23" s="69"/>
+      <c r="B23" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="65"/>
-    </row>
-    <row r="24" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="89" t="s">
+      <c r="C23" s="55"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="57"/>
+    </row>
+    <row r="24" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A24" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="56" t="s">
+      <c r="D24" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="56" t="s">
+      <c r="F24" s="39"/>
+      <c r="G24" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I24" s="73" t="s">
+      <c r="I24" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="67"/>
-      <c r="K24" s="56" t="s">
+      <c r="J24" s="46"/>
+      <c r="K24" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="22"/>
-      <c r="M24" s="52"/>
-    </row>
-    <row r="25" spans="1:13" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="90"/>
-      <c r="B25" s="31" t="s">
+      <c r="L24" s="36"/>
+      <c r="M24" s="49"/>
+    </row>
+    <row r="25" spans="1:13" ht="76.5" thickTop="1" thickBot="1">
+      <c r="A25" s="73"/>
+      <c r="B25" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="25" t="s">
+      <c r="C25" s="51"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="20" t="s">
+      <c r="F25" s="39"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I25" s="48"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="64"/>
-    </row>
-    <row r="26" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="90"/>
-      <c r="B26" s="9" t="s">
+      <c r="I25" s="74"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="54"/>
+    </row>
+    <row r="26" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A26" s="73"/>
+      <c r="B26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="25" t="s">
+      <c r="C26" s="51"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="20" t="s">
+      <c r="F26" s="39"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="48"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="64"/>
-    </row>
-    <row r="27" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="91"/>
-      <c r="B27" s="9" t="s">
+      <c r="I26" s="74"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="54"/>
+    </row>
+    <row r="27" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A27" s="75"/>
+      <c r="B27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="25" t="s">
+      <c r="C27" s="55"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="20" t="s">
+      <c r="F27" s="39"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I27" s="74"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="65"/>
-    </row>
-    <row r="28" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="83" t="s">
+      <c r="I27" s="76"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="57"/>
+    </row>
+    <row r="28" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A28" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="57"/>
-      <c r="G28" s="56" t="s">
+      <c r="F28" s="45"/>
+      <c r="G28" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="46" t="s">
+      <c r="H28" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="85" t="s">
+      <c r="I28" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="J28" s="87" t="s">
+      <c r="J28" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="K28" s="56" t="s">
+      <c r="K28" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="L28" s="22"/>
-      <c r="M28" s="52"/>
-    </row>
-    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
-      <c r="B29" s="79"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="65"/>
-    </row>
-    <row r="30" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="71" t="s">
+      <c r="L28" s="36"/>
+      <c r="M28" s="49"/>
+    </row>
+    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A29" s="40"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="83"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="57"/>
+    </row>
+    <row r="30" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A30" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="C30" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="57"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="46" t="s">
+      <c r="F30" s="45"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="56" t="s">
+      <c r="I30" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56" t="s">
+      <c r="J30" s="48"/>
+      <c r="K30" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="L30" s="22"/>
-      <c r="M30" s="52"/>
-    </row>
-    <row r="31" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="66"/>
-      <c r="B31" s="31" t="s">
+      <c r="L30" s="36"/>
+      <c r="M30" s="49"/>
+    </row>
+    <row r="31" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A31" s="85"/>
+      <c r="B31" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="25" t="s">
+      <c r="C31" s="51"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="57"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="64"/>
-    </row>
-    <row r="32" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="66"/>
-      <c r="B32" s="31" t="s">
+      <c r="F31" s="45"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="54"/>
+    </row>
+    <row r="32" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A32" s="85"/>
+      <c r="B32" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="25" t="s">
+      <c r="C32" s="51"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="57"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="64"/>
-    </row>
-    <row r="33" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
-      <c r="B33" s="9" t="s">
+      <c r="F32" s="45"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="54"/>
+    </row>
+    <row r="33" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A33" s="85"/>
+      <c r="B33" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="25" t="s">
+      <c r="C33" s="51"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="57"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="65"/>
-    </row>
-    <row r="34" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72"/>
-      <c r="B34" s="9" t="s">
+      <c r="F33" s="45"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="57"/>
+    </row>
+    <row r="34" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A34" s="86"/>
+      <c r="B34" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="68"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="25" t="s">
+      <c r="C34" s="55"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="57"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="29"/>
-    </row>
-    <row r="35" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="71" t="s">
+      <c r="F34" s="45"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="44"/>
+    </row>
+    <row r="35" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A35" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="67" t="s">
+      <c r="C35" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="56" t="s">
+      <c r="D35" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F35" s="57"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="46" t="s">
+      <c r="F35" s="45"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I35" s="56" t="s">
+      <c r="I35" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56" t="s">
+      <c r="J35" s="48"/>
+      <c r="K35" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="L35" s="22"/>
-      <c r="M35" s="52"/>
-    </row>
-    <row r="36" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
-      <c r="B36" s="9" t="s">
+      <c r="L35" s="36"/>
+      <c r="M35" s="49"/>
+    </row>
+    <row r="36" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A36" s="85"/>
+      <c r="B36" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="25" t="s">
+      <c r="C36" s="51"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="64"/>
-    </row>
-    <row r="37" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="72"/>
-      <c r="B37" s="9" t="s">
+      <c r="F36" s="45"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="54"/>
+    </row>
+    <row r="37" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A37" s="86"/>
+      <c r="B37" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="25" t="s">
+      <c r="C37" s="55"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
-      <c r="K37" s="62"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="65"/>
-    </row>
-    <row r="38" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="71" t="s">
+      <c r="F37" s="45"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="57"/>
+    </row>
+    <row r="38" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A38" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="67" t="s">
+      <c r="C38" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D38" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="57"/>
-      <c r="G38" s="56" t="s">
+      <c r="F38" s="45"/>
+      <c r="G38" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="46" t="s">
+      <c r="H38" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="48" t="s">
+      <c r="I38" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="J38" s="49"/>
-      <c r="K38" s="44" t="s">
+      <c r="J38" s="51"/>
+      <c r="K38" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="L38" s="22"/>
-      <c r="M38" s="52"/>
-    </row>
-    <row r="39" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="66"/>
-      <c r="B39" s="31" t="s">
+      <c r="L38" s="36"/>
+      <c r="M38" s="49"/>
+    </row>
+    <row r="39" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
+      <c r="A39" s="85"/>
+      <c r="B39" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="25" t="s">
+      <c r="C39" s="51"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="57"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="64"/>
-    </row>
-    <row r="40" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="66"/>
-      <c r="B40" s="9" t="s">
+      <c r="F39" s="45"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="54"/>
+    </row>
+    <row r="40" spans="1:13" ht="61.5" thickTop="1" thickBot="1">
+      <c r="A40" s="85"/>
+      <c r="B40" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="25" t="s">
+      <c r="C40" s="51"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="F40" s="57"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="64"/>
-    </row>
-    <row r="41" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="66"/>
-      <c r="B41" s="9" t="s">
+      <c r="F40" s="45"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="54"/>
+    </row>
+    <row r="41" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A41" s="85"/>
+      <c r="B41" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="25" t="s">
+      <c r="C41" s="51"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="57"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="64"/>
-    </row>
-    <row r="42" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="72"/>
-      <c r="B42" s="9" t="s">
+      <c r="F41" s="45"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="54"/>
+    </row>
+    <row r="42" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A42" s="86"/>
+      <c r="B42" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="68"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="25" t="s">
+      <c r="C42" s="55"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="57"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="57"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="65"/>
-    </row>
-    <row r="43" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="83" t="s">
+      <c r="F42" s="45"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="36"/>
+      <c r="M42" s="57"/>
+    </row>
+    <row r="43" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A43" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="67" t="s">
+      <c r="C43" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="56" t="s">
+      <c r="D43" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="56" t="s">
+      <c r="E43" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="F43" s="57"/>
-      <c r="G43" s="56" t="s">
+      <c r="F43" s="45"/>
+      <c r="G43" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="80"/>
-      <c r="J43" s="67" t="s">
+      <c r="I43" s="59"/>
+      <c r="J43" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="K43" s="56" t="s">
+      <c r="K43" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="L43" s="22"/>
-      <c r="M43" s="52"/>
-    </row>
-    <row r="44" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="84"/>
-      <c r="B44" s="31" t="s">
+      <c r="L43" s="36"/>
+      <c r="M43" s="49"/>
+    </row>
+    <row r="44" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
+      <c r="A44" s="40"/>
+      <c r="B44" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="68"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="81"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="62"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="65"/>
-    </row>
-    <row r="45" spans="1:13" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="71" t="s">
+      <c r="C44" s="55"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="57"/>
+    </row>
+    <row r="45" spans="1:13" ht="61.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A45" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="44" t="s">
+      <c r="D45" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="56" t="s">
+      <c r="E45" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="F45" s="57"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="46" t="s">
+      <c r="F45" s="45"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I45" s="44" t="s">
+      <c r="I45" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="J45" s="82"/>
-      <c r="K45" s="64" t="s">
+      <c r="J45" s="61"/>
+      <c r="K45" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="L45" s="22"/>
-      <c r="M45" s="52"/>
-    </row>
-    <row r="46" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="66"/>
-      <c r="B46" s="31" t="s">
+      <c r="L45" s="36"/>
+      <c r="M45" s="49"/>
+    </row>
+    <row r="46" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A46" s="85"/>
+      <c r="B46" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="64"/>
-    </row>
-    <row r="47" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="66"/>
-      <c r="B47" s="9" t="s">
+      <c r="C46" s="51"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="54"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="54"/>
+    </row>
+    <row r="47" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A47" s="85"/>
+      <c r="B47" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C47" s="49"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="64"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="64"/>
-    </row>
-    <row r="48" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="72"/>
-      <c r="B48" s="9" t="s">
+      <c r="C47" s="51"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="54"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="54"/>
+    </row>
+    <row r="48" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A48" s="86"/>
+      <c r="B48" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="62"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="57"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="64"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="65"/>
-    </row>
-    <row r="49" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="71" t="s">
+      <c r="C48" s="51"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="53"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="54"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="57"/>
+    </row>
+    <row r="49" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A49" s="84" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="78" t="s">
+      <c r="B49" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="67" t="s">
+      <c r="C49" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="56" t="s">
+      <c r="D49" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="56" t="s">
+      <c r="E49" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="F49" s="57"/>
-      <c r="G49" s="56" t="s">
+      <c r="F49" s="45"/>
+      <c r="G49" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="46" t="s">
+      <c r="H49" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I49" s="80"/>
-      <c r="J49" s="67" t="s">
+      <c r="I49" s="59"/>
+      <c r="J49" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="K49" s="52" t="s">
+      <c r="K49" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="L49" s="22"/>
-      <c r="M49" s="52"/>
-    </row>
-    <row r="50" spans="1:13" ht="104.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="72"/>
-      <c r="B50" s="79"/>
-      <c r="C50" s="68"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="62"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="81"/>
-      <c r="J50" s="68"/>
-      <c r="K50" s="65"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="65"/>
-    </row>
-    <row r="51" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="71" t="s">
+      <c r="L49" s="36"/>
+      <c r="M49" s="49"/>
+    </row>
+    <row r="50" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A50" s="86"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="57"/>
+    </row>
+    <row r="51" spans="1:13" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A51" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="44" t="s">
+      <c r="D51" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="E51" s="56" t="s">
+      <c r="E51" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="F51" s="57"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="46" t="s">
+      <c r="F51" s="45"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I51" s="44"/>
-      <c r="J51" s="44" t="s">
+      <c r="I51" s="53"/>
+      <c r="J51" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="K51" s="44" t="s">
+      <c r="K51" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="L51" s="22"/>
-      <c r="M51" s="52"/>
-    </row>
-    <row r="52" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="66"/>
-      <c r="B52" s="9" t="s">
+      <c r="L51" s="36"/>
+      <c r="M51" s="49"/>
+    </row>
+    <row r="52" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A52" s="85"/>
+      <c r="B52" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="49"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="64"/>
-    </row>
-    <row r="53" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="72"/>
-      <c r="B53" s="9" t="s">
+      <c r="C52" s="51"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="53"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="54"/>
+    </row>
+    <row r="53" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A53" s="86"/>
+      <c r="B53" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="68"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="62"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="57"/>
-      <c r="I53" s="62"/>
-      <c r="J53" s="62"/>
-      <c r="K53" s="62"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="65"/>
-    </row>
-    <row r="54" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="71" t="s">
+      <c r="C53" s="55"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="63"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="63"/>
+      <c r="K53" s="63"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="57"/>
+    </row>
+    <row r="54" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A54" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="C54" s="67" t="s">
+      <c r="C54" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="56" t="s">
+      <c r="D54" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="E54" s="56" t="s">
+      <c r="E54" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="F54" s="57"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="46" t="s">
+      <c r="F54" s="45"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I54" s="56" t="s">
+      <c r="I54" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="J54" s="56"/>
-      <c r="K54" s="56" t="s">
+      <c r="J54" s="48"/>
+      <c r="K54" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="L54" s="22"/>
-      <c r="M54" s="52"/>
-    </row>
-    <row r="55" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="66"/>
-      <c r="B55" s="31" t="s">
+      <c r="L54" s="36"/>
+      <c r="M54" s="49"/>
+    </row>
+    <row r="55" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
+      <c r="A55" s="85"/>
+      <c r="B55" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="49"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="57"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="44"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="64"/>
-    </row>
-    <row r="56" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="66"/>
-      <c r="B56" s="9" t="s">
+      <c r="C55" s="51"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+      <c r="L55" s="36"/>
+      <c r="M55" s="54"/>
+    </row>
+    <row r="56" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A56" s="85"/>
+      <c r="B56" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C56" s="49"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="57"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="64"/>
-    </row>
-    <row r="57" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="72"/>
-      <c r="B57" s="9" t="s">
+      <c r="C56" s="51"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="53"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="54"/>
+    </row>
+    <row r="57" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A57" s="86"/>
+      <c r="B57" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="68"/>
-      <c r="D57" s="62"/>
-      <c r="E57" s="62"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="62"/>
-      <c r="H57" s="57"/>
-      <c r="I57" s="62"/>
-      <c r="J57" s="62"/>
-      <c r="K57" s="62"/>
-      <c r="L57" s="22"/>
-      <c r="M57" s="65"/>
-    </row>
-    <row r="58" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="71" t="s">
+      <c r="C57" s="55"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="63"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="63"/>
+      <c r="J57" s="63"/>
+      <c r="K57" s="63"/>
+      <c r="L57" s="36"/>
+      <c r="M57" s="57"/>
+    </row>
+    <row r="58" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A58" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="67" t="s">
+      <c r="C58" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="56" t="s">
+      <c r="D58" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="E58" s="56" t="s">
+      <c r="E58" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="F58" s="57"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="46" t="s">
+      <c r="F58" s="45"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I58" s="73" t="s">
+      <c r="I58" s="72" t="s">
         <v>131</v>
       </c>
-      <c r="J58" s="34"/>
-      <c r="K58" s="56" t="s">
+      <c r="J58" s="87"/>
+      <c r="K58" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="L58" s="22"/>
-      <c r="M58" s="52"/>
-    </row>
-    <row r="59" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="66"/>
-      <c r="B59" s="31" t="s">
+      <c r="L58" s="36"/>
+      <c r="M58" s="49"/>
+    </row>
+    <row r="59" spans="1:13" ht="46.5" thickTop="1" thickBot="1">
+      <c r="A59" s="85"/>
+      <c r="B59" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="49"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="57"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="57"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="44"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="64"/>
-    </row>
-    <row r="60" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="66"/>
-      <c r="B60" s="9" t="s">
+      <c r="C59" s="51"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="74"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="53"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="54"/>
+    </row>
+    <row r="60" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A60" s="85"/>
+      <c r="B60" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C60" s="49"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="44"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="44"/>
-      <c r="H60" s="57"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="44"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="64"/>
-    </row>
-    <row r="61" spans="1:13" ht="107.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="72"/>
-      <c r="B61" s="9" t="s">
+      <c r="C60" s="51"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="74"/>
+      <c r="J60" s="88"/>
+      <c r="K60" s="53"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="54"/>
+    </row>
+    <row r="61" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A61" s="86"/>
+      <c r="B61" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="68"/>
-      <c r="D61" s="62"/>
-      <c r="E61" s="62"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="57"/>
-      <c r="I61" s="74"/>
-      <c r="J61" s="36"/>
-      <c r="K61" s="62"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="65"/>
-    </row>
-    <row r="62" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="71" t="s">
+      <c r="C61" s="55"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="76"/>
+      <c r="J61" s="89"/>
+      <c r="K61" s="63"/>
+      <c r="L61" s="36"/>
+      <c r="M61" s="57"/>
+    </row>
+    <row r="62" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A62" s="84" t="s">
         <v>134</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="C62" s="67" t="s">
+      <c r="C62" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D62" s="75" t="s">
+      <c r="D62" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="E62" s="56" t="s">
+      <c r="E62" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="F62" s="57"/>
-      <c r="G62" s="56" t="s">
+      <c r="F62" s="45"/>
+      <c r="G62" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="H62" s="46" t="s">
+      <c r="H62" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I62" s="73" t="s">
+      <c r="I62" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="J62" s="67"/>
-      <c r="K62" s="56" t="s">
+      <c r="J62" s="46"/>
+      <c r="K62" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="L62" s="22"/>
-      <c r="M62" s="52"/>
-    </row>
-    <row r="63" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="66"/>
-      <c r="B63" s="37" t="s">
+      <c r="L62" s="36"/>
+      <c r="M62" s="49"/>
+    </row>
+    <row r="63" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A63" s="85"/>
+      <c r="B63" s="91" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="49"/>
-      <c r="D63" s="76"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="57"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="57"/>
-      <c r="I63" s="48"/>
-      <c r="J63" s="49"/>
-      <c r="K63" s="44"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="64"/>
-    </row>
-    <row r="64" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="66"/>
-      <c r="B64" s="9" t="s">
+      <c r="C63" s="51"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="74"/>
+      <c r="J63" s="51"/>
+      <c r="K63" s="53"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="54"/>
+    </row>
+    <row r="64" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A64" s="85"/>
+      <c r="B64" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C64" s="49"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="44"/>
-      <c r="H64" s="57"/>
-      <c r="I64" s="48"/>
-      <c r="J64" s="49"/>
-      <c r="K64" s="44"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="64"/>
-    </row>
-    <row r="65" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="72"/>
-      <c r="B65" s="9" t="s">
+      <c r="C64" s="51"/>
+      <c r="D64" s="92"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="74"/>
+      <c r="J64" s="51"/>
+      <c r="K64" s="53"/>
+      <c r="L64" s="36"/>
+      <c r="M64" s="54"/>
+    </row>
+    <row r="65" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A65" s="86"/>
+      <c r="B65" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C65" s="68"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="62"/>
-      <c r="F65" s="57"/>
-      <c r="G65" s="62"/>
-      <c r="H65" s="57"/>
-      <c r="I65" s="74"/>
-      <c r="J65" s="68"/>
-      <c r="K65" s="62"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="65"/>
-    </row>
-    <row r="66" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="71" t="s">
+      <c r="C65" s="55"/>
+      <c r="D65" s="93"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="76"/>
+      <c r="J65" s="55"/>
+      <c r="K65" s="63"/>
+      <c r="L65" s="36"/>
+      <c r="M65" s="57"/>
+    </row>
+    <row r="66" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A66" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="C66" s="67" t="s">
+      <c r="C66" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="56" t="s">
+      <c r="D66" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="E66" s="56" t="s">
+      <c r="E66" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="F66" s="57"/>
-      <c r="G66" s="56" t="s">
+      <c r="F66" s="45"/>
+      <c r="G66" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="H66" s="46" t="s">
+      <c r="H66" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I66" s="73" t="s">
+      <c r="I66" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="J66" s="67"/>
-      <c r="K66" s="56" t="s">
+      <c r="J66" s="46"/>
+      <c r="K66" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="L66" s="22"/>
-      <c r="M66" s="52"/>
-    </row>
-    <row r="67" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="66"/>
-      <c r="B67" s="31" t="s">
+      <c r="L66" s="36"/>
+      <c r="M66" s="49"/>
+    </row>
+    <row r="67" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A67" s="85"/>
+      <c r="B67" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C67" s="49"/>
-      <c r="D67" s="44"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="57"/>
-      <c r="G67" s="44"/>
-      <c r="H67" s="57"/>
-      <c r="I67" s="48"/>
-      <c r="J67" s="49"/>
-      <c r="K67" s="44"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="64"/>
-    </row>
-    <row r="68" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="66"/>
-      <c r="B68" s="9" t="s">
+      <c r="C67" s="51"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="53"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="74"/>
+      <c r="J67" s="51"/>
+      <c r="K67" s="53"/>
+      <c r="L67" s="36"/>
+      <c r="M67" s="54"/>
+    </row>
+    <row r="68" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A68" s="85"/>
+      <c r="B68" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C68" s="49"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="57"/>
-      <c r="G68" s="44"/>
-      <c r="H68" s="57"/>
-      <c r="I68" s="48"/>
-      <c r="J68" s="49"/>
-      <c r="K68" s="44"/>
-      <c r="L68" s="22"/>
-      <c r="M68" s="64"/>
-    </row>
-    <row r="69" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="72"/>
-      <c r="B69" s="9" t="s">
+      <c r="C68" s="51"/>
+      <c r="D68" s="53"/>
+      <c r="E68" s="53"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="53"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="74"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="53"/>
+      <c r="L68" s="36"/>
+      <c r="M68" s="54"/>
+    </row>
+    <row r="69" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A69" s="86"/>
+      <c r="B69" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C69" s="68"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="57"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="57"/>
-      <c r="I69" s="74"/>
-      <c r="J69" s="68"/>
-      <c r="K69" s="62"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="65"/>
-    </row>
-    <row r="70" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="71" t="s">
+      <c r="C69" s="55"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="57"/>
+    </row>
+    <row r="70" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A70" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="31" t="s">
+      <c r="B70" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="C70" s="67" t="s">
+      <c r="C70" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D70" s="56" t="s">
+      <c r="D70" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="E70" s="56" t="s">
+      <c r="E70" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="F70" s="57"/>
-      <c r="G70" s="56" t="s">
+      <c r="F70" s="45"/>
+      <c r="G70" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="H70" s="46" t="s">
+      <c r="H70" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I70" s="73" t="s">
+      <c r="I70" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="J70" s="67"/>
-      <c r="K70" s="56" t="s">
+      <c r="J70" s="46"/>
+      <c r="K70" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="L70" s="22"/>
-      <c r="M70" s="52"/>
-    </row>
-    <row r="71" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="66"/>
-      <c r="B71" s="31" t="s">
+      <c r="L70" s="36"/>
+      <c r="M70" s="49"/>
+    </row>
+    <row r="71" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A71" s="85"/>
+      <c r="B71" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="49"/>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="44"/>
-      <c r="H71" s="57"/>
-      <c r="I71" s="48"/>
-      <c r="J71" s="49"/>
-      <c r="K71" s="44"/>
-      <c r="L71" s="22"/>
-      <c r="M71" s="64"/>
-    </row>
-    <row r="72" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="66"/>
-      <c r="B72" s="9" t="s">
+      <c r="C71" s="51"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="45"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="74"/>
+      <c r="J71" s="51"/>
+      <c r="K71" s="53"/>
+      <c r="L71" s="36"/>
+      <c r="M71" s="54"/>
+    </row>
+    <row r="72" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A72" s="85"/>
+      <c r="B72" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C72" s="49"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="57"/>
-      <c r="I72" s="48"/>
-      <c r="J72" s="49"/>
-      <c r="K72" s="44"/>
-      <c r="L72" s="22"/>
-      <c r="M72" s="64"/>
-    </row>
-    <row r="73" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="72"/>
-      <c r="B73" s="9" t="s">
+      <c r="C72" s="51"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="45"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="45"/>
+      <c r="I72" s="74"/>
+      <c r="J72" s="51"/>
+      <c r="K72" s="53"/>
+      <c r="L72" s="36"/>
+      <c r="M72" s="54"/>
+    </row>
+    <row r="73" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A73" s="86"/>
+      <c r="B73" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C73" s="68"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="62"/>
-      <c r="F73" s="57"/>
-      <c r="G73" s="62"/>
-      <c r="H73" s="57"/>
-      <c r="I73" s="74"/>
-      <c r="J73" s="68"/>
-      <c r="K73" s="62"/>
-      <c r="L73" s="22"/>
-      <c r="M73" s="65"/>
-    </row>
-    <row r="74" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="71" t="s">
+      <c r="C73" s="55"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="45"/>
+      <c r="G73" s="63"/>
+      <c r="H73" s="45"/>
+      <c r="I73" s="76"/>
+      <c r="J73" s="55"/>
+      <c r="K73" s="63"/>
+      <c r="L73" s="36"/>
+      <c r="M73" s="57"/>
+    </row>
+    <row r="74" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A74" s="84" t="s">
         <v>155</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="B74" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="C74" s="67" t="s">
+      <c r="C74" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D74" s="56" t="s">
+      <c r="D74" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="E74" s="56" t="s">
+      <c r="E74" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="F74" s="57"/>
-      <c r="G74" s="56"/>
-      <c r="H74" s="46" t="s">
+      <c r="F74" s="45"/>
+      <c r="G74" s="48"/>
+      <c r="H74" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I74" s="56" t="s">
+      <c r="I74" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="J74" s="56"/>
-      <c r="K74" s="56" t="s">
+      <c r="J74" s="48"/>
+      <c r="K74" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="L74" s="22"/>
-      <c r="M74" s="52"/>
-    </row>
-    <row r="75" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="66"/>
-      <c r="B75" s="31" t="s">
+      <c r="L74" s="36"/>
+      <c r="M74" s="49"/>
+    </row>
+    <row r="75" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A75" s="85"/>
+      <c r="B75" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C75" s="49"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="57"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="57"/>
-      <c r="I75" s="44"/>
-      <c r="J75" s="44"/>
-      <c r="K75" s="44"/>
-      <c r="L75" s="22"/>
-      <c r="M75" s="64"/>
-    </row>
-    <row r="76" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="66"/>
-      <c r="B76" s="31" t="s">
+      <c r="C75" s="51"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="45"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
+      <c r="L75" s="36"/>
+      <c r="M75" s="54"/>
+    </row>
+    <row r="76" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A76" s="85"/>
+      <c r="B76" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="C76" s="49"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="57"/>
-      <c r="G76" s="44"/>
-      <c r="H76" s="57"/>
-      <c r="I76" s="44"/>
-      <c r="J76" s="44"/>
-      <c r="K76" s="44"/>
-      <c r="L76" s="22"/>
-      <c r="M76" s="64"/>
-    </row>
-    <row r="77" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="66"/>
-      <c r="B77" s="9" t="s">
+      <c r="C76" s="51"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="45"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="53"/>
+      <c r="K76" s="53"/>
+      <c r="L76" s="36"/>
+      <c r="M76" s="54"/>
+    </row>
+    <row r="77" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A77" s="85"/>
+      <c r="B77" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C77" s="49"/>
-      <c r="D77" s="44"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="57"/>
-      <c r="G77" s="44"/>
-      <c r="H77" s="57"/>
-      <c r="I77" s="44"/>
-      <c r="J77" s="44"/>
-      <c r="K77" s="44"/>
-      <c r="L77" s="22"/>
-      <c r="M77" s="64"/>
-    </row>
-    <row r="78" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="72"/>
-      <c r="B78" s="9" t="s">
+      <c r="C77" s="51"/>
+      <c r="D77" s="53"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="45"/>
+      <c r="G77" s="53"/>
+      <c r="H77" s="45"/>
+      <c r="I77" s="53"/>
+      <c r="J77" s="53"/>
+      <c r="K77" s="53"/>
+      <c r="L77" s="36"/>
+      <c r="M77" s="54"/>
+    </row>
+    <row r="78" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A78" s="86"/>
+      <c r="B78" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="68"/>
-      <c r="D78" s="62"/>
-      <c r="E78" s="62"/>
-      <c r="F78" s="57"/>
-      <c r="G78" s="62"/>
-      <c r="H78" s="57"/>
-      <c r="I78" s="62"/>
-      <c r="J78" s="62"/>
-      <c r="K78" s="62"/>
-      <c r="L78" s="22"/>
-      <c r="M78" s="65"/>
-    </row>
-    <row r="79" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="71" t="s">
+      <c r="C78" s="55"/>
+      <c r="D78" s="63"/>
+      <c r="E78" s="63"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="63"/>
+      <c r="H78" s="45"/>
+      <c r="I78" s="63"/>
+      <c r="J78" s="63"/>
+      <c r="K78" s="63"/>
+      <c r="L78" s="36"/>
+      <c r="M78" s="57"/>
+    </row>
+    <row r="79" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A79" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="31" t="s">
+      <c r="B79" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="C79" s="67" t="s">
+      <c r="C79" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D79" s="56" t="s">
+      <c r="D79" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="E79" s="56" t="s">
+      <c r="E79" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="F79" s="57"/>
-      <c r="G79" s="56"/>
-      <c r="H79" s="46" t="s">
+      <c r="F79" s="45"/>
+      <c r="G79" s="48"/>
+      <c r="H79" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I79" s="56" t="s">
+      <c r="I79" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="J79" s="56"/>
-      <c r="K79" s="56" t="s">
+      <c r="J79" s="48"/>
+      <c r="K79" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="L79" s="22"/>
-      <c r="M79" s="52"/>
-    </row>
-    <row r="80" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="66"/>
-      <c r="B80" s="31" t="s">
+      <c r="L79" s="36"/>
+      <c r="M79" s="49"/>
+    </row>
+    <row r="80" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A80" s="85"/>
+      <c r="B80" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C80" s="49"/>
-      <c r="D80" s="44"/>
-      <c r="E80" s="44"/>
-      <c r="F80" s="57"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="57"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="44"/>
-      <c r="K80" s="44"/>
-      <c r="L80" s="22"/>
-      <c r="M80" s="64"/>
-    </row>
-    <row r="81" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="66"/>
-      <c r="B81" s="31" t="s">
+      <c r="C80" s="51"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="53"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="53"/>
+      <c r="H80" s="45"/>
+      <c r="I80" s="53"/>
+      <c r="J80" s="53"/>
+      <c r="K80" s="53"/>
+      <c r="L80" s="36"/>
+      <c r="M80" s="54"/>
+    </row>
+    <row r="81" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A81" s="85"/>
+      <c r="B81" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C81" s="49"/>
-      <c r="D81" s="44"/>
-      <c r="E81" s="44"/>
-      <c r="F81" s="57"/>
-      <c r="G81" s="44"/>
-      <c r="H81" s="57"/>
-      <c r="I81" s="44"/>
-      <c r="J81" s="44"/>
-      <c r="K81" s="44"/>
-      <c r="L81" s="22"/>
-      <c r="M81" s="64"/>
-    </row>
-    <row r="82" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="66"/>
-      <c r="B82" s="9" t="s">
+      <c r="C81" s="51"/>
+      <c r="D81" s="53"/>
+      <c r="E81" s="53"/>
+      <c r="F81" s="45"/>
+      <c r="G81" s="53"/>
+      <c r="H81" s="45"/>
+      <c r="I81" s="53"/>
+      <c r="J81" s="53"/>
+      <c r="K81" s="53"/>
+      <c r="L81" s="36"/>
+      <c r="M81" s="54"/>
+    </row>
+    <row r="82" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A82" s="85"/>
+      <c r="B82" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C82" s="49"/>
-      <c r="D82" s="44"/>
-      <c r="E82" s="44"/>
-      <c r="F82" s="57"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="57"/>
-      <c r="I82" s="44"/>
-      <c r="J82" s="44"/>
-      <c r="K82" s="44"/>
-      <c r="L82" s="22"/>
-      <c r="M82" s="64"/>
-    </row>
-    <row r="83" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="72"/>
-      <c r="B83" s="9" t="s">
+      <c r="C82" s="51"/>
+      <c r="D82" s="53"/>
+      <c r="E82" s="53"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="53"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="53"/>
+      <c r="J82" s="53"/>
+      <c r="K82" s="53"/>
+      <c r="L82" s="36"/>
+      <c r="M82" s="54"/>
+    </row>
+    <row r="83" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A83" s="86"/>
+      <c r="B83" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C83" s="68"/>
-      <c r="D83" s="62"/>
-      <c r="E83" s="62"/>
-      <c r="F83" s="57"/>
-      <c r="G83" s="62"/>
-      <c r="H83" s="57"/>
-      <c r="I83" s="62"/>
-      <c r="J83" s="62"/>
-      <c r="K83" s="62"/>
-      <c r="L83" s="22"/>
-      <c r="M83" s="65"/>
-    </row>
-    <row r="84" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="71" t="s">
+      <c r="C83" s="55"/>
+      <c r="D83" s="63"/>
+      <c r="E83" s="63"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="63"/>
+      <c r="H83" s="45"/>
+      <c r="I83" s="63"/>
+      <c r="J83" s="63"/>
+      <c r="K83" s="63"/>
+      <c r="L83" s="36"/>
+      <c r="M83" s="57"/>
+    </row>
+    <row r="84" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A84" s="84" t="s">
         <v>167</v>
       </c>
-      <c r="B84" s="31" t="s">
+      <c r="B84" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="C84" s="67" t="s">
+      <c r="C84" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D84" s="56" t="s">
+      <c r="D84" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E84" s="56" t="s">
+      <c r="E84" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="F84" s="57"/>
-      <c r="G84" s="56"/>
-      <c r="H84" s="46" t="s">
+      <c r="F84" s="45"/>
+      <c r="G84" s="48"/>
+      <c r="H84" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I84" s="56" t="s">
+      <c r="I84" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="J84" s="56"/>
-      <c r="K84" s="56" t="s">
+      <c r="J84" s="48"/>
+      <c r="K84" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="L84" s="22"/>
-      <c r="M84" s="52"/>
-    </row>
-    <row r="85" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="66"/>
-      <c r="B85" s="31" t="s">
+      <c r="L84" s="36"/>
+      <c r="M84" s="49"/>
+    </row>
+    <row r="85" spans="1:13" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A85" s="85"/>
+      <c r="B85" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="C85" s="49"/>
-      <c r="D85" s="44"/>
-      <c r="E85" s="44"/>
-      <c r="F85" s="57"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="57"/>
-      <c r="I85" s="44"/>
-      <c r="J85" s="44"/>
-      <c r="K85" s="44"/>
-      <c r="L85" s="22"/>
-      <c r="M85" s="64"/>
-    </row>
-    <row r="86" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="66"/>
-      <c r="B86" s="9" t="s">
+      <c r="C85" s="51"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="45"/>
+      <c r="G85" s="53"/>
+      <c r="H85" s="45"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
+      <c r="L85" s="36"/>
+      <c r="M85" s="54"/>
+    </row>
+    <row r="86" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A86" s="85"/>
+      <c r="B86" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C86" s="49"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="57"/>
-      <c r="G86" s="44"/>
-      <c r="H86" s="57"/>
-      <c r="I86" s="44"/>
-      <c r="J86" s="44"/>
-      <c r="K86" s="44"/>
-      <c r="L86" s="22"/>
-      <c r="M86" s="64"/>
-    </row>
-    <row r="87" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="55"/>
-      <c r="B87" s="9" t="s">
+      <c r="C86" s="51"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="53"/>
+      <c r="H86" s="45"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="53"/>
+      <c r="K86" s="53"/>
+      <c r="L86" s="36"/>
+      <c r="M86" s="54"/>
+    </row>
+    <row r="87" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A87" s="94"/>
+      <c r="B87" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C87" s="68"/>
-      <c r="D87" s="62"/>
-      <c r="E87" s="62"/>
-      <c r="F87" s="57"/>
-      <c r="G87" s="62"/>
-      <c r="H87" s="57"/>
-      <c r="I87" s="62"/>
-      <c r="J87" s="62"/>
-      <c r="K87" s="62"/>
-      <c r="L87" s="22"/>
-      <c r="M87" s="65"/>
-    </row>
-    <row r="88" spans="1:13" ht="136.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="54" t="s">
+      <c r="C87" s="55"/>
+      <c r="D87" s="63"/>
+      <c r="E87" s="63"/>
+      <c r="F87" s="45"/>
+      <c r="G87" s="63"/>
+      <c r="H87" s="45"/>
+      <c r="I87" s="63"/>
+      <c r="J87" s="63"/>
+      <c r="K87" s="63"/>
+      <c r="L87" s="36"/>
+      <c r="M87" s="57"/>
+    </row>
+    <row r="88" spans="1:13" ht="136.5" thickTop="1" thickBot="1">
+      <c r="A88" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C88" s="67" t="s">
+      <c r="C88" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D88" s="56" t="s">
+      <c r="D88" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="E88" s="56" t="s">
+      <c r="E88" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="F88" s="57"/>
-      <c r="G88" s="56"/>
-      <c r="H88" s="46" t="s">
+      <c r="F88" s="45"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I88" s="30"/>
-      <c r="J88" s="38"/>
-      <c r="K88" s="56" t="s">
+      <c r="I88" s="47"/>
+      <c r="J88" s="96"/>
+      <c r="K88" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="L88" s="22"/>
-      <c r="M88" s="52"/>
-    </row>
-    <row r="89" spans="1:13" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="66"/>
-      <c r="B89" s="9" t="s">
+      <c r="L88" s="36"/>
+      <c r="M88" s="49"/>
+    </row>
+    <row r="89" spans="1:13" ht="106.5" thickTop="1" thickBot="1">
+      <c r="A89" s="85"/>
+      <c r="B89" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="49"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="44"/>
-      <c r="F89" s="57"/>
-      <c r="G89" s="44"/>
-      <c r="H89" s="57"/>
-      <c r="I89" s="32"/>
-      <c r="J89" s="39"/>
-      <c r="K89" s="44"/>
-      <c r="L89" s="22"/>
-      <c r="M89" s="64"/>
-    </row>
-    <row r="90" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="58" t="s">
+      <c r="C89" s="51"/>
+      <c r="D89" s="53"/>
+      <c r="E89" s="53"/>
+      <c r="F89" s="45"/>
+      <c r="G89" s="53"/>
+      <c r="H89" s="45"/>
+      <c r="I89" s="52"/>
+      <c r="J89" s="97"/>
+      <c r="K89" s="53"/>
+      <c r="L89" s="36"/>
+      <c r="M89" s="54"/>
+    </row>
+    <row r="90" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A90" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="40" t="s">
+      <c r="B90" s="99" t="s">
         <v>178</v>
       </c>
-      <c r="C90" s="49"/>
-      <c r="D90" s="44"/>
-      <c r="E90" s="44"/>
-      <c r="F90" s="57"/>
-      <c r="G90" s="44"/>
-      <c r="H90" s="57"/>
-      <c r="I90" s="60" t="s">
+      <c r="C90" s="51"/>
+      <c r="D90" s="53"/>
+      <c r="E90" s="53"/>
+      <c r="F90" s="45"/>
+      <c r="G90" s="53"/>
+      <c r="H90" s="45"/>
+      <c r="I90" s="100" t="s">
         <v>179</v>
       </c>
-      <c r="J90" s="39"/>
-      <c r="K90" s="44"/>
-      <c r="L90" s="22"/>
-      <c r="M90" s="64"/>
-    </row>
-    <row r="91" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="59"/>
-      <c r="B91" s="40" t="s">
+      <c r="J90" s="97"/>
+      <c r="K90" s="53"/>
+      <c r="L90" s="36"/>
+      <c r="M90" s="54"/>
+    </row>
+    <row r="91" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A91" s="101"/>
+      <c r="B91" s="99" t="s">
         <v>148</v>
       </c>
-      <c r="C91" s="49"/>
-      <c r="D91" s="44"/>
-      <c r="E91" s="44"/>
-      <c r="F91" s="57"/>
-      <c r="G91" s="44"/>
-      <c r="H91" s="57"/>
-      <c r="I91" s="61"/>
-      <c r="J91" s="39"/>
-      <c r="K91" s="44"/>
-      <c r="L91" s="22"/>
-      <c r="M91" s="64"/>
-    </row>
-    <row r="92" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="58" t="s">
+      <c r="C91" s="51"/>
+      <c r="D91" s="53"/>
+      <c r="E91" s="53"/>
+      <c r="F91" s="45"/>
+      <c r="G91" s="53"/>
+      <c r="H91" s="45"/>
+      <c r="I91" s="102"/>
+      <c r="J91" s="97"/>
+      <c r="K91" s="53"/>
+      <c r="L91" s="36"/>
+      <c r="M91" s="54"/>
+    </row>
+    <row r="92" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A92" s="98" t="s">
         <v>180</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="C92" s="49"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="57"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="57"/>
-      <c r="I92" s="60" t="s">
+      <c r="C92" s="51"/>
+      <c r="D92" s="53"/>
+      <c r="E92" s="53"/>
+      <c r="F92" s="45"/>
+      <c r="G92" s="53"/>
+      <c r="H92" s="45"/>
+      <c r="I92" s="100" t="s">
         <v>182</v>
       </c>
-      <c r="J92" s="39"/>
-      <c r="K92" s="44"/>
-      <c r="L92" s="22"/>
-      <c r="M92" s="64"/>
-    </row>
-    <row r="93" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="59"/>
-      <c r="B93" s="31" t="s">
+      <c r="J92" s="97"/>
+      <c r="K92" s="53"/>
+      <c r="L92" s="36"/>
+      <c r="M92" s="54"/>
+    </row>
+    <row r="93" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A93" s="101"/>
+      <c r="B93" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C93" s="49"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="44"/>
-      <c r="F93" s="57"/>
-      <c r="G93" s="44"/>
-      <c r="H93" s="57"/>
-      <c r="I93" s="61"/>
-      <c r="J93" s="39"/>
-      <c r="K93" s="44"/>
-      <c r="L93" s="22"/>
-      <c r="M93" s="64"/>
-    </row>
-    <row r="94" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="58" t="s">
+      <c r="C93" s="51"/>
+      <c r="D93" s="53"/>
+      <c r="E93" s="53"/>
+      <c r="F93" s="45"/>
+      <c r="G93" s="53"/>
+      <c r="H93" s="45"/>
+      <c r="I93" s="102"/>
+      <c r="J93" s="97"/>
+      <c r="K93" s="53"/>
+      <c r="L93" s="36"/>
+      <c r="M93" s="54"/>
+    </row>
+    <row r="94" spans="1:13" ht="31.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A94" s="98" t="s">
         <v>183</v>
       </c>
-      <c r="B94" s="31" t="s">
+      <c r="B94" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="C94" s="49"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="44"/>
-      <c r="F94" s="57"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="57"/>
-      <c r="I94" s="69" t="s">
+      <c r="C94" s="51"/>
+      <c r="D94" s="53"/>
+      <c r="E94" s="53"/>
+      <c r="F94" s="45"/>
+      <c r="G94" s="53"/>
+      <c r="H94" s="45"/>
+      <c r="I94" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="J94" s="39"/>
-      <c r="K94" s="44"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="64"/>
-    </row>
-    <row r="95" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="59"/>
-      <c r="B95" s="31" t="s">
+      <c r="J94" s="97"/>
+      <c r="K94" s="53"/>
+      <c r="L94" s="36"/>
+      <c r="M94" s="54"/>
+    </row>
+    <row r="95" spans="1:13" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A95" s="101"/>
+      <c r="B95" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C95" s="49"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="44"/>
-      <c r="F95" s="57"/>
-      <c r="G95" s="44"/>
-      <c r="H95" s="57"/>
-      <c r="I95" s="70"/>
-      <c r="J95" s="39"/>
-      <c r="K95" s="44"/>
-      <c r="L95" s="22"/>
-      <c r="M95" s="64"/>
-    </row>
-    <row r="96" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="58" t="s">
+      <c r="C95" s="51"/>
+      <c r="D95" s="53"/>
+      <c r="E95" s="53"/>
+      <c r="F95" s="45"/>
+      <c r="G95" s="53"/>
+      <c r="H95" s="45"/>
+      <c r="I95" s="104"/>
+      <c r="J95" s="97"/>
+      <c r="K95" s="53"/>
+      <c r="L95" s="36"/>
+      <c r="M95" s="54"/>
+    </row>
+    <row r="96" spans="1:13" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A96" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="B96" s="31" t="s">
+      <c r="B96" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="C96" s="49"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="44"/>
-      <c r="F96" s="57"/>
-      <c r="G96" s="44"/>
-      <c r="H96" s="57"/>
-      <c r="I96" s="60" t="s">
+      <c r="C96" s="51"/>
+      <c r="D96" s="53"/>
+      <c r="E96" s="53"/>
+      <c r="F96" s="45"/>
+      <c r="G96" s="53"/>
+      <c r="H96" s="45"/>
+      <c r="I96" s="100" t="s">
         <v>188</v>
       </c>
-      <c r="J96" s="39"/>
-      <c r="K96" s="44"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="64"/>
-    </row>
-    <row r="97" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="59"/>
-      <c r="B97" s="31" t="s">
+      <c r="J96" s="97"/>
+      <c r="K96" s="53"/>
+      <c r="L96" s="36"/>
+      <c r="M96" s="54"/>
+    </row>
+    <row r="97" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A97" s="101"/>
+      <c r="B97" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C97" s="49"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="44"/>
-      <c r="F97" s="57"/>
-      <c r="G97" s="44"/>
-      <c r="H97" s="57"/>
-      <c r="I97" s="61"/>
-      <c r="J97" s="39"/>
-      <c r="K97" s="44"/>
-      <c r="L97" s="22"/>
-      <c r="M97" s="64"/>
-    </row>
-    <row r="98" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="58" t="s">
+      <c r="C97" s="51"/>
+      <c r="D97" s="53"/>
+      <c r="E97" s="53"/>
+      <c r="F97" s="45"/>
+      <c r="G97" s="53"/>
+      <c r="H97" s="45"/>
+      <c r="I97" s="102"/>
+      <c r="J97" s="97"/>
+      <c r="K97" s="53"/>
+      <c r="L97" s="36"/>
+      <c r="M97" s="54"/>
+    </row>
+    <row r="98" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A98" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="B98" s="31" t="s">
+      <c r="B98" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="C98" s="49"/>
-      <c r="D98" s="44"/>
-      <c r="E98" s="44"/>
-      <c r="F98" s="57"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="57"/>
-      <c r="I98" s="60" t="s">
+      <c r="C98" s="51"/>
+      <c r="D98" s="53"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="45"/>
+      <c r="G98" s="53"/>
+      <c r="H98" s="45"/>
+      <c r="I98" s="100" t="s">
         <v>191</v>
       </c>
-      <c r="J98" s="39"/>
-      <c r="K98" s="44"/>
-      <c r="L98" s="22"/>
-      <c r="M98" s="64"/>
-    </row>
-    <row r="99" spans="1:13" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="59"/>
-      <c r="B99" s="31" t="s">
+      <c r="J98" s="97"/>
+      <c r="K98" s="53"/>
+      <c r="L98" s="36"/>
+      <c r="M98" s="54"/>
+    </row>
+    <row r="99" spans="1:13" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A99" s="101"/>
+      <c r="B99" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C99" s="49"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="44"/>
-      <c r="F99" s="57"/>
-      <c r="G99" s="44"/>
-      <c r="H99" s="57"/>
-      <c r="I99" s="61"/>
-      <c r="J99" s="39"/>
-      <c r="K99" s="44"/>
-      <c r="L99" s="22"/>
-      <c r="M99" s="64"/>
-    </row>
-    <row r="100" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="58" t="s">
+      <c r="C99" s="51"/>
+      <c r="D99" s="53"/>
+      <c r="E99" s="53"/>
+      <c r="F99" s="45"/>
+      <c r="G99" s="53"/>
+      <c r="H99" s="45"/>
+      <c r="I99" s="102"/>
+      <c r="J99" s="97"/>
+      <c r="K99" s="53"/>
+      <c r="L99" s="36"/>
+      <c r="M99" s="54"/>
+    </row>
+    <row r="100" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A100" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="B100" s="31" t="s">
+      <c r="B100" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="C100" s="49"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="44"/>
-      <c r="F100" s="57"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="57"/>
-      <c r="I100" s="60" t="s">
+      <c r="C100" s="51"/>
+      <c r="D100" s="53"/>
+      <c r="E100" s="53"/>
+      <c r="F100" s="45"/>
+      <c r="G100" s="53"/>
+      <c r="H100" s="45"/>
+      <c r="I100" s="100" t="s">
         <v>194</v>
       </c>
-      <c r="J100" s="39"/>
-      <c r="K100" s="44"/>
-      <c r="L100" s="22"/>
-      <c r="M100" s="64"/>
-    </row>
-    <row r="101" spans="1:13" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="59"/>
-      <c r="B101" s="31" t="s">
+      <c r="J100" s="97"/>
+      <c r="K100" s="53"/>
+      <c r="L100" s="36"/>
+      <c r="M100" s="54"/>
+    </row>
+    <row r="101" spans="1:13" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A101" s="101"/>
+      <c r="B101" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="C101" s="49"/>
-      <c r="D101" s="44"/>
-      <c r="E101" s="44"/>
-      <c r="F101" s="57"/>
-      <c r="G101" s="44"/>
-      <c r="H101" s="57"/>
-      <c r="I101" s="63"/>
-      <c r="J101" s="39"/>
-      <c r="K101" s="44"/>
-      <c r="L101" s="22"/>
-      <c r="M101" s="64"/>
-    </row>
-    <row r="102" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="58" t="s">
+      <c r="C101" s="51"/>
+      <c r="D101" s="53"/>
+      <c r="E101" s="53"/>
+      <c r="F101" s="45"/>
+      <c r="G101" s="53"/>
+      <c r="H101" s="45"/>
+      <c r="I101" s="105"/>
+      <c r="J101" s="97"/>
+      <c r="K101" s="53"/>
+      <c r="L101" s="36"/>
+      <c r="M101" s="54"/>
+    </row>
+    <row r="102" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A102" s="98" t="s">
         <v>195</v>
       </c>
-      <c r="B102" s="31" t="s">
+      <c r="B102" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="C102" s="49"/>
-      <c r="D102" s="44"/>
-      <c r="E102" s="44"/>
-      <c r="F102" s="57"/>
-      <c r="G102" s="44"/>
-      <c r="H102" s="57"/>
-      <c r="I102" s="60" t="s">
+      <c r="C102" s="51"/>
+      <c r="D102" s="53"/>
+      <c r="E102" s="53"/>
+      <c r="F102" s="45"/>
+      <c r="G102" s="53"/>
+      <c r="H102" s="45"/>
+      <c r="I102" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="J102" s="39"/>
-      <c r="K102" s="44"/>
-      <c r="L102" s="22"/>
-      <c r="M102" s="64"/>
-    </row>
-    <row r="103" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="59"/>
-      <c r="B103" s="31" t="s">
+      <c r="J102" s="97"/>
+      <c r="K102" s="53"/>
+      <c r="L102" s="36"/>
+      <c r="M102" s="54"/>
+    </row>
+    <row r="103" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A103" s="101"/>
+      <c r="B103" s="50" t="s">
         <v>198</v>
       </c>
-      <c r="C103" s="49"/>
-      <c r="D103" s="44"/>
-      <c r="E103" s="44"/>
-      <c r="F103" s="57"/>
-      <c r="G103" s="44"/>
-      <c r="H103" s="57"/>
-      <c r="I103" s="61"/>
-      <c r="J103" s="39"/>
-      <c r="K103" s="44"/>
-      <c r="L103" s="22"/>
-      <c r="M103" s="64"/>
-    </row>
-    <row r="104" spans="1:13" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="58" t="s">
+      <c r="C103" s="51"/>
+      <c r="D103" s="53"/>
+      <c r="E103" s="53"/>
+      <c r="F103" s="45"/>
+      <c r="G103" s="53"/>
+      <c r="H103" s="45"/>
+      <c r="I103" s="102"/>
+      <c r="J103" s="97"/>
+      <c r="K103" s="53"/>
+      <c r="L103" s="36"/>
+      <c r="M103" s="54"/>
+    </row>
+    <row r="104" spans="1:13" ht="28.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A104" s="98" t="s">
         <v>199</v>
       </c>
-      <c r="B104" s="31" t="s">
+      <c r="B104" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="C104" s="49"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="44"/>
-      <c r="F104" s="57"/>
-      <c r="G104" s="44"/>
-      <c r="H104" s="57"/>
-      <c r="I104" s="60" t="s">
+      <c r="C104" s="51"/>
+      <c r="D104" s="53"/>
+      <c r="E104" s="53"/>
+      <c r="F104" s="45"/>
+      <c r="G104" s="53"/>
+      <c r="H104" s="45"/>
+      <c r="I104" s="100" t="s">
         <v>201</v>
       </c>
-      <c r="J104" s="39"/>
-      <c r="K104" s="44"/>
-      <c r="L104" s="22"/>
-      <c r="M104" s="64"/>
-    </row>
-    <row r="105" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="59"/>
-      <c r="B105" s="31" t="s">
+      <c r="J104" s="97"/>
+      <c r="K104" s="53"/>
+      <c r="L104" s="36"/>
+      <c r="M104" s="54"/>
+    </row>
+    <row r="105" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A105" s="101"/>
+      <c r="B105" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="C105" s="49"/>
-      <c r="D105" s="44"/>
-      <c r="E105" s="44"/>
-      <c r="F105" s="57"/>
-      <c r="G105" s="44"/>
-      <c r="H105" s="57"/>
-      <c r="I105" s="61"/>
-      <c r="J105" s="39"/>
-      <c r="K105" s="44"/>
-      <c r="L105" s="22"/>
-      <c r="M105" s="64"/>
-    </row>
-    <row r="106" spans="1:13" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="58" t="s">
+      <c r="C105" s="51"/>
+      <c r="D105" s="53"/>
+      <c r="E105" s="53"/>
+      <c r="F105" s="45"/>
+      <c r="G105" s="53"/>
+      <c r="H105" s="45"/>
+      <c r="I105" s="102"/>
+      <c r="J105" s="97"/>
+      <c r="K105" s="53"/>
+      <c r="L105" s="36"/>
+      <c r="M105" s="54"/>
+    </row>
+    <row r="106" spans="1:13" ht="27.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A106" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="B106" s="31" t="s">
+      <c r="B106" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="C106" s="49"/>
-      <c r="D106" s="44"/>
-      <c r="E106" s="44"/>
-      <c r="F106" s="57"/>
-      <c r="G106" s="44"/>
-      <c r="H106" s="57"/>
-      <c r="I106" s="60" t="s">
+      <c r="C106" s="51"/>
+      <c r="D106" s="53"/>
+      <c r="E106" s="53"/>
+      <c r="F106" s="45"/>
+      <c r="G106" s="53"/>
+      <c r="H106" s="45"/>
+      <c r="I106" s="100" t="s">
         <v>205</v>
       </c>
-      <c r="J106" s="39"/>
-      <c r="K106" s="44"/>
-      <c r="L106" s="22"/>
-      <c r="M106" s="64"/>
-    </row>
-    <row r="107" spans="1:13" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="59"/>
-      <c r="B107" s="31" t="s">
+      <c r="J106" s="97"/>
+      <c r="K106" s="53"/>
+      <c r="L106" s="36"/>
+      <c r="M106" s="54"/>
+    </row>
+    <row r="107" spans="1:13" ht="18" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A107" s="101"/>
+      <c r="B107" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="C107" s="68"/>
-      <c r="D107" s="62"/>
-      <c r="E107" s="62"/>
-      <c r="F107" s="57"/>
-      <c r="G107" s="62"/>
-      <c r="H107" s="57"/>
-      <c r="I107" s="62"/>
-      <c r="J107" s="41"/>
-      <c r="K107" s="62"/>
-      <c r="L107" s="22"/>
-      <c r="M107" s="65"/>
-    </row>
-    <row r="108" spans="1:13" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="54" t="s">
+      <c r="C107" s="55"/>
+      <c r="D107" s="63"/>
+      <c r="E107" s="63"/>
+      <c r="F107" s="45"/>
+      <c r="G107" s="63"/>
+      <c r="H107" s="45"/>
+      <c r="I107" s="63"/>
+      <c r="J107" s="106"/>
+      <c r="K107" s="63"/>
+      <c r="L107" s="36"/>
+      <c r="M107" s="57"/>
+    </row>
+    <row r="108" spans="1:13" ht="22.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A108" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="B108" s="31" t="s">
+      <c r="B108" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="C108" s="49" t="s">
+      <c r="C108" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D108" s="44" t="s">
+      <c r="D108" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="E108" s="56" t="s">
+      <c r="E108" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="F108" s="57"/>
-      <c r="G108" s="44" t="s">
+      <c r="F108" s="45"/>
+      <c r="G108" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="H108" s="46" t="s">
+      <c r="H108" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="I108" s="48" t="s">
+      <c r="I108" s="74" t="s">
         <v>210</v>
       </c>
-      <c r="J108" s="49"/>
-      <c r="K108" s="44" t="s">
+      <c r="J108" s="51"/>
+      <c r="K108" s="53" t="s">
         <v>211</v>
       </c>
-      <c r="L108" s="22"/>
-      <c r="M108" s="52"/>
-    </row>
-    <row r="109" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="55"/>
-      <c r="B109" s="42" t="s">
+      <c r="L108" s="36"/>
+      <c r="M108" s="49"/>
+    </row>
+    <row r="109" spans="1:13" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A109" s="94"/>
+      <c r="B109" s="107" t="s">
         <v>212</v>
       </c>
-      <c r="C109" s="51"/>
-      <c r="D109" s="45"/>
-      <c r="E109" s="45"/>
-      <c r="F109" s="47"/>
-      <c r="G109" s="45"/>
-      <c r="H109" s="47"/>
-      <c r="I109" s="50"/>
-      <c r="J109" s="51"/>
-      <c r="K109" s="45"/>
-      <c r="L109" s="43"/>
-      <c r="M109" s="53"/>
+      <c r="C109" s="108"/>
+      <c r="D109" s="109"/>
+      <c r="E109" s="109"/>
+      <c r="F109" s="110"/>
+      <c r="G109" s="109"/>
+      <c r="H109" s="110"/>
+      <c r="I109" s="111"/>
+      <c r="J109" s="108"/>
+      <c r="K109" s="109"/>
+      <c r="L109" s="112"/>
+      <c r="M109" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="251">
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="K11:K14"/>
-    <mergeCell ref="M11:M14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="J15:J19"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="M15:M19"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="I24:J27"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="M24:M27"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="G30:G34"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="I30:I34"/>
-    <mergeCell ref="J30:J34"/>
-    <mergeCell ref="K30:K34"/>
-    <mergeCell ref="M30:M33"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="K35:K37"/>
-    <mergeCell ref="M35:M37"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H38:H42"/>
-    <mergeCell ref="I38:J42"/>
-    <mergeCell ref="K38:K42"/>
-    <mergeCell ref="M38:M42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="F38:F42"/>
-    <mergeCell ref="G38:G42"/>
-    <mergeCell ref="M45:M48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="K49:K50"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="G45:G48"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="I45:I48"/>
-    <mergeCell ref="J45:J48"/>
-    <mergeCell ref="K45:K48"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="M51:M53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="G54:G57"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="I54:I57"/>
-    <mergeCell ref="J54:J57"/>
-    <mergeCell ref="K54:K57"/>
-    <mergeCell ref="M54:M57"/>
-    <mergeCell ref="G51:G53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="K51:K53"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="I58:I61"/>
-    <mergeCell ref="K58:K61"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="H62:H65"/>
-    <mergeCell ref="I62:J65"/>
-    <mergeCell ref="K62:K65"/>
-    <mergeCell ref="M62:M65"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="G66:G69"/>
-    <mergeCell ref="H66:H69"/>
-    <mergeCell ref="I66:J69"/>
-    <mergeCell ref="K66:K69"/>
-    <mergeCell ref="M66:M69"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="G70:G73"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="I70:J73"/>
-    <mergeCell ref="K70:K73"/>
-    <mergeCell ref="M70:M73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="H108:H109"/>
+    <mergeCell ref="I108:J109"/>
+    <mergeCell ref="K108:K109"/>
+    <mergeCell ref="M108:M109"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="I102:I103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="I96:I97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="M84:M87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="C88:C107"/>
+    <mergeCell ref="D88:D107"/>
+    <mergeCell ref="E88:E107"/>
+    <mergeCell ref="F88:F107"/>
+    <mergeCell ref="G88:G107"/>
+    <mergeCell ref="H88:H107"/>
+    <mergeCell ref="K88:K107"/>
+    <mergeCell ref="M88:M107"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="I90:I91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="I92:I93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="I94:I95"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="H84:H87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
     <mergeCell ref="E84:E87"/>
     <mergeCell ref="F84:F87"/>
     <mergeCell ref="M74:M78"/>
@@ -6351,52 +6214,187 @@
     <mergeCell ref="D74:D78"/>
     <mergeCell ref="E74:E78"/>
     <mergeCell ref="F74:F78"/>
-    <mergeCell ref="M84:M87"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="C88:C107"/>
-    <mergeCell ref="D88:D107"/>
-    <mergeCell ref="E88:E107"/>
-    <mergeCell ref="F88:F107"/>
-    <mergeCell ref="G88:G107"/>
-    <mergeCell ref="H88:H107"/>
-    <mergeCell ref="K88:K107"/>
-    <mergeCell ref="M88:M107"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="I90:I91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="I92:I93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="I94:I95"/>
-    <mergeCell ref="G84:G87"/>
-    <mergeCell ref="H84:H87"/>
-    <mergeCell ref="I84:I87"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="K84:K87"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="I102:I103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="I96:I97"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="I98:I99"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="H108:H109"/>
-    <mergeCell ref="I108:J109"/>
-    <mergeCell ref="K108:K109"/>
-    <mergeCell ref="M108:M109"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="I70:J73"/>
+    <mergeCell ref="K70:K73"/>
+    <mergeCell ref="M70:M73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="I66:J69"/>
+    <mergeCell ref="K66:K69"/>
+    <mergeCell ref="M66:M69"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="H62:H65"/>
+    <mergeCell ref="I62:J65"/>
+    <mergeCell ref="K62:K65"/>
+    <mergeCell ref="M62:M65"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="I58:I61"/>
+    <mergeCell ref="K58:K61"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="M51:M53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="I54:I57"/>
+    <mergeCell ref="J54:J57"/>
+    <mergeCell ref="K54:K57"/>
+    <mergeCell ref="M54:M57"/>
+    <mergeCell ref="G51:G53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="K51:K53"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="M45:M48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="K49:K50"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="G45:G48"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="I45:I48"/>
+    <mergeCell ref="J45:J48"/>
+    <mergeCell ref="K45:K48"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="H38:H42"/>
+    <mergeCell ref="I38:J42"/>
+    <mergeCell ref="K38:K42"/>
+    <mergeCell ref="M38:M42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="F38:F42"/>
+    <mergeCell ref="G38:G42"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="K35:K37"/>
+    <mergeCell ref="M35:M37"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="G30:G34"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="I30:I34"/>
+    <mergeCell ref="J30:J34"/>
+    <mergeCell ref="K30:K34"/>
+    <mergeCell ref="M30:M33"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="M20:M23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="I24:J27"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="M24:M27"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="K11:K14"/>
+    <mergeCell ref="M11:M14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="I15:I19"/>
+    <mergeCell ref="J15:J19"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="M15:M19"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6406,24 +6404,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>